<commit_message>
club master, desgina nd fix some codes
</commit_message>
<xml_diff>
--- a/Region 1 club details.xlsx
+++ b/Region 1 club details.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\live_project\lions_clubs_International\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03517B4A-8EFB-468D-B17E-5CC53286DB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6320"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="club in Region 1 - 3 zones" sheetId="2" r:id="rId1"/>
@@ -11766,7 +11767,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -11874,22 +11875,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12171,16 +12172,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12191,7 +12197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -12202,7 +12208,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -12213,7 +12219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -12224,7 +12230,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -12235,7 +12241,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -12246,7 +12252,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -12257,7 +12263,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -12268,7 +12274,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -12279,7 +12285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -12290,7 +12296,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>15</v>
       </c>
@@ -12301,7 +12307,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -12312,7 +12318,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -12323,7 +12329,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -12334,7 +12340,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>20</v>
       </c>
@@ -12345,7 +12351,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -12356,7 +12362,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>22</v>
       </c>
@@ -12373,22 +12379,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V494"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12454,7 +12460,7 @@
       </c>
       <c r="V1" s="7"/>
     </row>
-    <row r="3" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -12520,7 +12526,7 @@
       </c>
       <c r="V3" s="7"/>
     </row>
-    <row r="4" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" s="4" t="s">
         <v>4</v>
@@ -12584,7 +12590,7 @@
       </c>
       <c r="V4" s="7"/>
     </row>
-    <row r="5" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="4" t="s">
         <v>4</v>
@@ -12648,7 +12654,7 @@
       </c>
       <c r="V5" s="7"/>
     </row>
-    <row r="6" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="4" t="s">
         <v>4</v>
@@ -12712,7 +12718,7 @@
       </c>
       <c r="V6" s="7"/>
     </row>
-    <row r="7" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="8"/>
       <c r="B7" s="4" t="s">
         <v>4</v>
@@ -12776,7 +12782,7 @@
       </c>
       <c r="V7" s="7"/>
     </row>
-    <row r="8" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="8"/>
       <c r="B8" s="4" t="s">
         <v>4</v>
@@ -12840,7 +12846,7 @@
       </c>
       <c r="V8" s="7"/>
     </row>
-    <row r="9" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="4" t="s">
         <v>4</v>
@@ -12904,7 +12910,7 @@
       </c>
       <c r="V9" s="7"/>
     </row>
-    <row r="10" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
       <c r="B10" s="4" t="s">
         <v>4</v>
@@ -12968,7 +12974,7 @@
       </c>
       <c r="V10" s="7"/>
     </row>
-    <row r="11" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
       <c r="B11" s="4" t="s">
         <v>4</v>
@@ -13032,7 +13038,7 @@
       </c>
       <c r="V11" s="7"/>
     </row>
-    <row r="12" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
       <c r="B12" s="4" t="s">
         <v>4</v>
@@ -13096,7 +13102,7 @@
       </c>
       <c r="V12" s="7"/>
     </row>
-    <row r="13" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
       <c r="B13" s="4" t="s">
         <v>4</v>
@@ -13160,7 +13166,7 @@
       </c>
       <c r="V13" s="7"/>
     </row>
-    <row r="14" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
       <c r="B14" s="4" t="s">
         <v>4</v>
@@ -13224,7 +13230,7 @@
       </c>
       <c r="V14" s="7"/>
     </row>
-    <row r="15" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -13288,7 +13294,7 @@
       </c>
       <c r="V15" s="7"/>
     </row>
-    <row r="16" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
       <c r="B16" s="4" t="s">
         <v>4</v>
@@ -13352,7 +13358,7 @@
       </c>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
       <c r="B17" s="4" t="s">
         <v>4</v>
@@ -13416,7 +13422,7 @@
       </c>
       <c r="V17" s="7"/>
     </row>
-    <row r="18" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
       <c r="B18" s="4" t="s">
         <v>4</v>
@@ -13480,7 +13486,7 @@
       </c>
       <c r="V18" s="7"/>
     </row>
-    <row r="19" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="8"/>
       <c r="B19" s="4" t="s">
         <v>4</v>
@@ -13544,7 +13550,7 @@
       </c>
       <c r="V19" s="7"/>
     </row>
-    <row r="20" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="8"/>
       <c r="B20" s="4" t="s">
         <v>4</v>
@@ -13608,7 +13614,7 @@
       </c>
       <c r="V20" s="7"/>
     </row>
-    <row r="21" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="8"/>
       <c r="B21" s="4" t="s">
         <v>4</v>
@@ -13672,7 +13678,7 @@
       </c>
       <c r="V21" s="7"/>
     </row>
-    <row r="22" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="8"/>
       <c r="B22" s="4" t="s">
         <v>4</v>
@@ -13736,7 +13742,7 @@
       </c>
       <c r="V22" s="7"/>
     </row>
-    <row r="23" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="8"/>
       <c r="B23" s="4" t="s">
         <v>4</v>
@@ -13800,7 +13806,7 @@
       </c>
       <c r="V23" s="7"/>
     </row>
-    <row r="24" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="8"/>
       <c r="B24" s="4" t="s">
         <v>4</v>
@@ -13864,7 +13870,7 @@
       </c>
       <c r="V24" s="7"/>
     </row>
-    <row r="25" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="8"/>
       <c r="B25" s="4" t="s">
         <v>4</v>
@@ -13928,7 +13934,7 @@
       </c>
       <c r="V25" s="7"/>
     </row>
-    <row r="26" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="8"/>
       <c r="B26" s="4" t="s">
         <v>4</v>
@@ -13992,7 +13998,7 @@
       </c>
       <c r="V26" s="7"/>
     </row>
-    <row r="27" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="8"/>
       <c r="B27" s="4" t="s">
         <v>4</v>
@@ -14056,7 +14062,7 @@
       </c>
       <c r="V27" s="7"/>
     </row>
-    <row r="28" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="4" t="s">
         <v>4</v>
@@ -14120,7 +14126,7 @@
       </c>
       <c r="V28" s="7"/>
     </row>
-    <row r="29" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="8"/>
       <c r="B29" s="4" t="s">
         <v>4</v>
@@ -14184,7 +14190,7 @@
       </c>
       <c r="V29" s="7"/>
     </row>
-    <row r="30" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="8"/>
       <c r="B30" s="4" t="s">
         <v>4</v>
@@ -14248,7 +14254,7 @@
       </c>
       <c r="V30" s="7"/>
     </row>
-    <row r="31" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="8"/>
       <c r="B31" s="4" t="s">
         <v>4</v>
@@ -14312,7 +14318,7 @@
       </c>
       <c r="V31" s="7"/>
     </row>
-    <row r="32" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="8"/>
       <c r="B32" s="4" t="s">
         <v>4</v>
@@ -14376,7 +14382,7 @@
       </c>
       <c r="V32" s="7"/>
     </row>
-    <row r="33" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="8"/>
       <c r="B33" s="4" t="s">
         <v>4</v>
@@ -14440,7 +14446,7 @@
       </c>
       <c r="V33" s="7"/>
     </row>
-    <row r="34" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="8"/>
       <c r="B34" s="4" t="s">
         <v>4</v>
@@ -14504,7 +14510,7 @@
       </c>
       <c r="V34" s="7"/>
     </row>
-    <row r="35" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="8"/>
       <c r="B35" s="4" t="s">
         <v>4</v>
@@ -14568,7 +14574,7 @@
       </c>
       <c r="V35" s="7"/>
     </row>
-    <row r="36" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="8"/>
       <c r="B36" s="4" t="s">
         <v>4</v>
@@ -14632,7 +14638,7 @@
       </c>
       <c r="V36" s="7"/>
     </row>
-    <row r="37" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="8"/>
       <c r="B37" s="4" t="s">
         <v>4</v>
@@ -14696,7 +14702,7 @@
       </c>
       <c r="V37" s="7"/>
     </row>
-    <row r="38" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="8"/>
       <c r="B38" s="4" t="s">
         <v>4</v>
@@ -14760,7 +14766,7 @@
       </c>
       <c r="V38" s="7"/>
     </row>
-    <row r="39" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="8"/>
       <c r="B39" s="4" t="s">
         <v>4</v>
@@ -14824,7 +14830,7 @@
       </c>
       <c r="V39" s="7"/>
     </row>
-    <row r="40" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
       <c r="B40" s="4" t="s">
         <v>4</v>
@@ -14888,7 +14894,7 @@
       </c>
       <c r="V40" s="7"/>
     </row>
-    <row r="41" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
       <c r="B41" s="4" t="s">
         <v>4</v>
@@ -14952,7 +14958,7 @@
       </c>
       <c r="V41" s="7"/>
     </row>
-    <row r="42" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="8"/>
       <c r="B42" s="4" t="s">
         <v>4</v>
@@ -15016,7 +15022,7 @@
       </c>
       <c r="V42" s="7"/>
     </row>
-    <row r="43" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="8"/>
       <c r="B43" s="4" t="s">
         <v>4</v>
@@ -15080,7 +15086,7 @@
       </c>
       <c r="V43" s="7"/>
     </row>
-    <row r="44" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="8"/>
       <c r="B44" s="4" t="s">
         <v>4</v>
@@ -15144,7 +15150,7 @@
       </c>
       <c r="V44" s="7"/>
     </row>
-    <row r="45" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
       <c r="B45" s="4" t="s">
         <v>4</v>
@@ -15208,7 +15214,7 @@
       </c>
       <c r="V45" s="7"/>
     </row>
-    <row r="46" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="8"/>
       <c r="B46" s="4" t="s">
         <v>4</v>
@@ -15272,7 +15278,7 @@
       </c>
       <c r="V46" s="7"/>
     </row>
-    <row r="47" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="8"/>
       <c r="B47" s="4" t="s">
         <v>4</v>
@@ -15336,7 +15342,7 @@
       </c>
       <c r="V47" s="7"/>
     </row>
-    <row r="48" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="8"/>
       <c r="B48" s="4" t="s">
         <v>4</v>
@@ -15400,7 +15406,7 @@
       </c>
       <c r="V48" s="7"/>
     </row>
-    <row r="49" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="8"/>
       <c r="B49" s="4" t="s">
         <v>4</v>
@@ -15464,7 +15470,7 @@
       </c>
       <c r="V49" s="7"/>
     </row>
-    <row r="50" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="4" t="s">
         <v>4</v>
@@ -15528,7 +15534,7 @@
       </c>
       <c r="V50" s="7"/>
     </row>
-    <row r="51" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
       <c r="B51" s="4" t="s">
         <v>4</v>
@@ -15592,7 +15598,7 @@
       </c>
       <c r="V51" s="7"/>
     </row>
-    <row r="52" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="8"/>
       <c r="B52" s="4" t="s">
         <v>4</v>
@@ -15656,7 +15662,7 @@
       </c>
       <c r="V52" s="7"/>
     </row>
-    <row r="53" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="8"/>
       <c r="B53" s="4" t="s">
         <v>4</v>
@@ -15720,7 +15726,7 @@
       </c>
       <c r="V53" s="7"/>
     </row>
-    <row r="54" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="8"/>
       <c r="B54" s="4" t="s">
         <v>4</v>
@@ -15784,7 +15790,7 @@
       </c>
       <c r="V54" s="7"/>
     </row>
-    <row r="55" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="8"/>
       <c r="B55" s="4" t="s">
         <v>4</v>
@@ -15848,7 +15854,7 @@
       </c>
       <c r="V55" s="7"/>
     </row>
-    <row r="56" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
       <c r="B56" s="4" t="s">
         <v>4</v>
@@ -15912,7 +15918,7 @@
       </c>
       <c r="V56" s="7"/>
     </row>
-    <row r="57" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="8"/>
       <c r="B57" s="4" t="s">
         <v>4</v>
@@ -15976,7 +15982,7 @@
       </c>
       <c r="V57" s="7"/>
     </row>
-    <row r="58" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="8"/>
       <c r="B58" s="4" t="s">
         <v>4</v>
@@ -16040,7 +16046,7 @@
       </c>
       <c r="V58" s="7"/>
     </row>
-    <row r="59" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="8"/>
       <c r="B59" s="4" t="s">
         <v>4</v>
@@ -16104,7 +16110,7 @@
       </c>
       <c r="V59" s="7"/>
     </row>
-    <row r="60" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="8"/>
       <c r="B60" s="4" t="s">
         <v>4</v>
@@ -16168,7 +16174,7 @@
       </c>
       <c r="V60" s="7"/>
     </row>
-    <row r="61" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="8"/>
       <c r="B61" s="4" t="s">
         <v>4</v>
@@ -16232,7 +16238,7 @@
       </c>
       <c r="V61" s="7"/>
     </row>
-    <row r="62" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="8"/>
       <c r="B62" s="4" t="s">
         <v>4</v>
@@ -16296,7 +16302,7 @@
       </c>
       <c r="V62" s="7"/>
     </row>
-    <row r="63" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="8"/>
       <c r="B63" s="4" t="s">
         <v>4</v>
@@ -16360,7 +16366,7 @@
       </c>
       <c r="V63" s="7"/>
     </row>
-    <row r="64" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="8"/>
       <c r="B64" s="4" t="s">
         <v>4</v>
@@ -16424,7 +16430,7 @@
       </c>
       <c r="V64" s="7"/>
     </row>
-    <row r="65" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
       <c r="B65" s="4" t="s">
         <v>4</v>
@@ -16488,7 +16494,7 @@
       </c>
       <c r="V65" s="7"/>
     </row>
-    <row r="66" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="4" t="s">
         <v>4</v>
@@ -16552,7 +16558,7 @@
       </c>
       <c r="V66" s="7"/>
     </row>
-    <row r="67" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="8"/>
       <c r="B67" s="4" t="s">
         <v>4</v>
@@ -16616,7 +16622,7 @@
       </c>
       <c r="V67" s="7"/>
     </row>
-    <row r="68" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>8</v>
       </c>
@@ -16682,7 +16688,7 @@
       </c>
       <c r="V68" s="7"/>
     </row>
-    <row r="69" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="8"/>
       <c r="B69" s="4" t="s">
         <v>4</v>
@@ -16746,7 +16752,7 @@
       </c>
       <c r="V69" s="7"/>
     </row>
-    <row r="70" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
       <c r="B70" s="4" t="s">
         <v>4</v>
@@ -16810,7 +16816,7 @@
       </c>
       <c r="V70" s="7"/>
     </row>
-    <row r="71" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="4" t="s">
         <v>4</v>
@@ -16874,7 +16880,7 @@
       </c>
       <c r="V71" s="7"/>
     </row>
-    <row r="72" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="4" t="s">
         <v>4</v>
@@ -16938,7 +16944,7 @@
       </c>
       <c r="V72" s="7"/>
     </row>
-    <row r="73" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="4" t="s">
         <v>4</v>
@@ -17002,7 +17008,7 @@
       </c>
       <c r="V73" s="7"/>
     </row>
-    <row r="74" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="4" t="s">
         <v>4</v>
@@ -17066,7 +17072,7 @@
       </c>
       <c r="V74" s="7"/>
     </row>
-    <row r="75" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="8"/>
       <c r="B75" s="4" t="s">
         <v>4</v>
@@ -17130,7 +17136,7 @@
       </c>
       <c r="V75" s="7"/>
     </row>
-    <row r="76" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
       <c r="B76" s="4" t="s">
         <v>4</v>
@@ -17194,7 +17200,7 @@
       </c>
       <c r="V76" s="7"/>
     </row>
-    <row r="77" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="8"/>
       <c r="B77" s="4" t="s">
         <v>4</v>
@@ -17258,7 +17264,7 @@
       </c>
       <c r="V77" s="7"/>
     </row>
-    <row r="78" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
       <c r="B78" s="4" t="s">
         <v>4</v>
@@ -17322,7 +17328,7 @@
       </c>
       <c r="V78" s="7"/>
     </row>
-    <row r="79" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="4" t="s">
         <v>4</v>
@@ -17386,7 +17392,7 @@
       </c>
       <c r="V79" s="7"/>
     </row>
-    <row r="80" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
       <c r="B80" s="4" t="s">
         <v>4</v>
@@ -17450,7 +17456,7 @@
       </c>
       <c r="V80" s="7"/>
     </row>
-    <row r="81" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="4" t="s">
         <v>4</v>
@@ -17514,7 +17520,7 @@
       </c>
       <c r="V81" s="7"/>
     </row>
-    <row r="82" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>7</v>
       </c>
@@ -17580,7 +17586,7 @@
       </c>
       <c r="V82" s="7"/>
     </row>
-    <row r="83" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
       <c r="B83" s="4" t="s">
         <v>4</v>
@@ -17644,7 +17650,7 @@
       </c>
       <c r="V83" s="7"/>
     </row>
-    <row r="84" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" s="4" t="s">
         <v>4</v>
@@ -17708,7 +17714,7 @@
       </c>
       <c r="V84" s="7"/>
     </row>
-    <row r="85" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="4" t="s">
         <v>4</v>
@@ -17772,7 +17778,7 @@
       </c>
       <c r="V85" s="7"/>
     </row>
-    <row r="86" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="8"/>
       <c r="B86" s="4" t="s">
         <v>4</v>
@@ -17836,7 +17842,7 @@
       </c>
       <c r="V86" s="7"/>
     </row>
-    <row r="87" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="4" t="s">
         <v>4</v>
@@ -17900,7 +17906,7 @@
       </c>
       <c r="V87" s="7"/>
     </row>
-    <row r="88" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="4" t="s">
         <v>4</v>
@@ -17964,7 +17970,7 @@
       </c>
       <c r="V88" s="7"/>
     </row>
-    <row r="89" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="4" t="s">
         <v>4</v>
@@ -18028,7 +18034,7 @@
       </c>
       <c r="V89" s="7"/>
     </row>
-    <row r="90" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="4" t="s">
         <v>4</v>
@@ -18092,7 +18098,7 @@
       </c>
       <c r="V90" s="7"/>
     </row>
-    <row r="91" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="4" t="s">
         <v>4</v>
@@ -18156,7 +18162,7 @@
       </c>
       <c r="V91" s="7"/>
     </row>
-    <row r="92" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="8"/>
       <c r="B92" s="4" t="s">
         <v>4</v>
@@ -18220,7 +18226,7 @@
       </c>
       <c r="V92" s="7"/>
     </row>
-    <row r="93" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="4" t="s">
         <v>4</v>
@@ -18284,7 +18290,7 @@
       </c>
       <c r="V93" s="7"/>
     </row>
-    <row r="94" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
       <c r="B94" s="4" t="s">
         <v>4</v>
@@ -18348,7 +18354,7 @@
       </c>
       <c r="V94" s="7"/>
     </row>
-    <row r="95" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="4" t="s">
         <v>4</v>
@@ -18412,7 +18418,7 @@
       </c>
       <c r="V95" s="7"/>
     </row>
-    <row r="96" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="8"/>
       <c r="B96" s="4" t="s">
         <v>4</v>
@@ -18476,7 +18482,7 @@
       </c>
       <c r="V96" s="7"/>
     </row>
-    <row r="97" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
       <c r="B97" s="4" t="s">
         <v>4</v>
@@ -18540,7 +18546,7 @@
       </c>
       <c r="V97" s="7"/>
     </row>
-    <row r="98" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="4" t="s">
         <v>4</v>
@@ -18604,7 +18610,7 @@
       </c>
       <c r="V98" s="7"/>
     </row>
-    <row r="99" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="8"/>
       <c r="B99" s="4" t="s">
         <v>4</v>
@@ -18668,7 +18674,7 @@
       </c>
       <c r="V99" s="7"/>
     </row>
-    <row r="100" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="8"/>
       <c r="B100" s="4" t="s">
         <v>4</v>
@@ -18732,7 +18738,7 @@
       </c>
       <c r="V100" s="7"/>
     </row>
-    <row r="101" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="4" t="s">
         <v>4</v>
@@ -18796,7 +18802,7 @@
       </c>
       <c r="V101" s="7"/>
     </row>
-    <row r="102" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="8"/>
       <c r="B102" s="4" t="s">
         <v>4</v>
@@ -18860,7 +18866,7 @@
       </c>
       <c r="V102" s="7"/>
     </row>
-    <row r="103" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="8"/>
       <c r="B103" s="4" t="s">
         <v>4</v>
@@ -18924,7 +18930,7 @@
       </c>
       <c r="V103" s="7"/>
     </row>
-    <row r="104" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="8"/>
       <c r="B104" s="4" t="s">
         <v>4</v>
@@ -18988,7 +18994,7 @@
       </c>
       <c r="V104" s="7"/>
     </row>
-    <row r="105" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
       <c r="B105" s="4" t="s">
         <v>4</v>
@@ -19052,7 +19058,7 @@
       </c>
       <c r="V105" s="7"/>
     </row>
-    <row r="106" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="8"/>
       <c r="B106" s="4" t="s">
         <v>4</v>
@@ -19116,7 +19122,7 @@
       </c>
       <c r="V106" s="7"/>
     </row>
-    <row r="107" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
       <c r="B107" s="4" t="s">
         <v>4</v>
@@ -19180,7 +19186,7 @@
       </c>
       <c r="V107" s="7"/>
     </row>
-    <row r="108" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="8"/>
       <c r="B108" s="4" t="s">
         <v>4</v>
@@ -19244,7 +19250,7 @@
       </c>
       <c r="V108" s="7"/>
     </row>
-    <row r="109" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
       <c r="B109" s="4" t="s">
         <v>4</v>
@@ -19308,7 +19314,7 @@
       </c>
       <c r="V109" s="7"/>
     </row>
-    <row r="110" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="8"/>
       <c r="B110" s="4" t="s">
         <v>4</v>
@@ -19372,7 +19378,7 @@
       </c>
       <c r="V110" s="7"/>
     </row>
-    <row r="111" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="8"/>
       <c r="B111" s="4" t="s">
         <v>4</v>
@@ -19436,7 +19442,7 @@
       </c>
       <c r="V111" s="7"/>
     </row>
-    <row r="112" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="8"/>
       <c r="B112" s="4" t="s">
         <v>4</v>
@@ -19500,7 +19506,7 @@
       </c>
       <c r="V112" s="7"/>
     </row>
-    <row r="113" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="8"/>
       <c r="B113" s="4" t="s">
         <v>4</v>
@@ -19564,7 +19570,7 @@
       </c>
       <c r="V113" s="7"/>
     </row>
-    <row r="114" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="8"/>
       <c r="B114" s="4" t="s">
         <v>4</v>
@@ -19628,7 +19634,7 @@
       </c>
       <c r="V114" s="7"/>
     </row>
-    <row r="115" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="8"/>
       <c r="B115" s="4" t="s">
         <v>4</v>
@@ -19690,7 +19696,7 @@
       </c>
       <c r="V115" s="7"/>
     </row>
-    <row r="116" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="8"/>
       <c r="B116" s="4" t="s">
         <v>4</v>
@@ -19754,7 +19760,7 @@
       </c>
       <c r="V116" s="7"/>
     </row>
-    <row r="117" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="8"/>
       <c r="B117" s="4" t="s">
         <v>4</v>
@@ -19818,7 +19824,7 @@
       </c>
       <c r="V117" s="7"/>
     </row>
-    <row r="118" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>6</v>
       </c>
@@ -19884,7 +19890,7 @@
       </c>
       <c r="V118" s="7"/>
     </row>
-    <row r="119" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="8"/>
       <c r="B119" s="4" t="s">
         <v>4</v>
@@ -19948,7 +19954,7 @@
       </c>
       <c r="V119" s="7"/>
     </row>
-    <row r="120" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="8"/>
       <c r="B120" s="4" t="s">
         <v>4</v>
@@ -20012,7 +20018,7 @@
       </c>
       <c r="V120" s="7"/>
     </row>
-    <row r="121" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="8"/>
       <c r="B121" s="4" t="s">
         <v>4</v>
@@ -20076,7 +20082,7 @@
       </c>
       <c r="V121" s="7"/>
     </row>
-    <row r="122" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="8"/>
       <c r="B122" s="4" t="s">
         <v>4</v>
@@ -20140,7 +20146,7 @@
       </c>
       <c r="V122" s="7"/>
     </row>
-    <row r="123" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="8"/>
       <c r="B123" s="4" t="s">
         <v>4</v>
@@ -20204,7 +20210,7 @@
       </c>
       <c r="V123" s="7"/>
     </row>
-    <row r="124" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="8"/>
       <c r="B124" s="4" t="s">
         <v>4</v>
@@ -20268,7 +20274,7 @@
       </c>
       <c r="V124" s="7"/>
     </row>
-    <row r="125" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="8"/>
       <c r="B125" s="4" t="s">
         <v>4</v>
@@ -20332,7 +20338,7 @@
       </c>
       <c r="V125" s="7"/>
     </row>
-    <row r="126" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A126" s="8"/>
       <c r="B126" s="4" t="s">
         <v>4</v>
@@ -20396,7 +20402,7 @@
       </c>
       <c r="V126" s="7"/>
     </row>
-    <row r="127" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A127" s="8"/>
       <c r="B127" s="4" t="s">
         <v>4</v>
@@ -20460,7 +20466,7 @@
       </c>
       <c r="V127" s="7"/>
     </row>
-    <row r="128" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
       <c r="B128" s="4" t="s">
         <v>4</v>
@@ -20524,7 +20530,7 @@
       </c>
       <c r="V128" s="7"/>
     </row>
-    <row r="129" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A129" s="8"/>
       <c r="B129" s="4" t="s">
         <v>4</v>
@@ -20588,7 +20594,7 @@
       </c>
       <c r="V129" s="7"/>
     </row>
-    <row r="130" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A130" s="8"/>
       <c r="B130" s="4" t="s">
         <v>4</v>
@@ -20652,7 +20658,7 @@
       </c>
       <c r="V130" s="7"/>
     </row>
-    <row r="131" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A131" s="8"/>
       <c r="B131" s="4" t="s">
         <v>4</v>
@@ -20716,7 +20722,7 @@
       </c>
       <c r="V131" s="7"/>
     </row>
-    <row r="132" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A132" s="8"/>
       <c r="B132" s="4" t="s">
         <v>4</v>
@@ -20780,7 +20786,7 @@
       </c>
       <c r="V132" s="7"/>
     </row>
-    <row r="133" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A133" s="8"/>
       <c r="B133" s="4" t="s">
         <v>4</v>
@@ -20844,7 +20850,7 @@
       </c>
       <c r="V133" s="7"/>
     </row>
-    <row r="134" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A134" s="8"/>
       <c r="B134" s="4" t="s">
         <v>4</v>
@@ -20908,7 +20914,7 @@
       </c>
       <c r="V134" s="7"/>
     </row>
-    <row r="135" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A135" s="8"/>
       <c r="B135" s="4" t="s">
         <v>4</v>
@@ -20972,7 +20978,7 @@
       </c>
       <c r="V135" s="7"/>
     </row>
-    <row r="136" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A136" s="8"/>
       <c r="B136" s="4" t="s">
         <v>4</v>
@@ -21036,7 +21042,7 @@
       </c>
       <c r="V136" s="7"/>
     </row>
-    <row r="137" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A137" s="8"/>
       <c r="B137" s="4" t="s">
         <v>4</v>
@@ -21100,7 +21106,7 @@
       </c>
       <c r="V137" s="7"/>
     </row>
-    <row r="138" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A138" s="8"/>
       <c r="B138" s="4" t="s">
         <v>4</v>
@@ -21164,7 +21170,7 @@
       </c>
       <c r="V138" s="7"/>
     </row>
-    <row r="139" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A139" s="8"/>
       <c r="B139" s="4" t="s">
         <v>4</v>
@@ -21228,7 +21234,7 @@
       </c>
       <c r="V139" s="7"/>
     </row>
-    <row r="140" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A140" s="8"/>
       <c r="B140" s="4" t="s">
         <v>4</v>
@@ -21292,7 +21298,7 @@
       </c>
       <c r="V140" s="7"/>
     </row>
-    <row r="141" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141" s="8"/>
       <c r="B141" s="4" t="s">
         <v>4</v>
@@ -21356,7 +21362,7 @@
       </c>
       <c r="V141" s="7"/>
     </row>
-    <row r="142" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142" s="8"/>
       <c r="B142" s="4" t="s">
         <v>4</v>
@@ -21420,7 +21426,7 @@
       </c>
       <c r="V142" s="7"/>
     </row>
-    <row r="143" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="4" t="s">
         <v>4</v>
@@ -21484,7 +21490,7 @@
       </c>
       <c r="V143" s="7"/>
     </row>
-    <row r="144" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>3</v>
       </c>
@@ -21550,7 +21556,7 @@
       </c>
       <c r="V144" s="7"/>
     </row>
-    <row r="145" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145" s="8"/>
       <c r="B145" s="4" t="s">
         <v>4</v>
@@ -21614,7 +21620,7 @@
       </c>
       <c r="V145" s="7"/>
     </row>
-    <row r="146" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A146" s="8"/>
       <c r="B146" s="4" t="s">
         <v>4</v>
@@ -21678,7 +21684,7 @@
       </c>
       <c r="V146" s="7"/>
     </row>
-    <row r="147" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A147" s="8"/>
       <c r="B147" s="4" t="s">
         <v>4</v>
@@ -21742,7 +21748,7 @@
       </c>
       <c r="V147" s="7"/>
     </row>
-    <row r="148" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A148" s="8"/>
       <c r="B148" s="4" t="s">
         <v>4</v>
@@ -21806,7 +21812,7 @@
       </c>
       <c r="V148" s="7"/>
     </row>
-    <row r="149" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A149" s="8"/>
       <c r="B149" s="4" t="s">
         <v>4</v>
@@ -21870,7 +21876,7 @@
       </c>
       <c r="V149" s="7"/>
     </row>
-    <row r="150" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A150" s="8"/>
       <c r="B150" s="4" t="s">
         <v>4</v>
@@ -21934,7 +21940,7 @@
       </c>
       <c r="V150" s="7"/>
     </row>
-    <row r="151" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A151" s="8"/>
       <c r="B151" s="4" t="s">
         <v>4</v>
@@ -21998,7 +22004,7 @@
       </c>
       <c r="V151" s="7"/>
     </row>
-    <row r="152" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A152" s="8"/>
       <c r="B152" s="4" t="s">
         <v>4</v>
@@ -22062,7 +22068,7 @@
       </c>
       <c r="V152" s="7"/>
     </row>
-    <row r="153" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A153" s="8"/>
       <c r="B153" s="4" t="s">
         <v>4</v>
@@ -22126,7 +22132,7 @@
       </c>
       <c r="V153" s="7"/>
     </row>
-    <row r="154" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A154" s="8"/>
       <c r="B154" s="4" t="s">
         <v>4</v>
@@ -22190,7 +22196,7 @@
       </c>
       <c r="V154" s="7"/>
     </row>
-    <row r="155" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A155" s="8"/>
       <c r="B155" s="4" t="s">
         <v>4</v>
@@ -22254,7 +22260,7 @@
       </c>
       <c r="V155" s="7"/>
     </row>
-    <row r="156" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A156" s="8"/>
       <c r="B156" s="4" t="s">
         <v>4</v>
@@ -22318,7 +22324,7 @@
       </c>
       <c r="V156" s="7"/>
     </row>
-    <row r="157" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A157" s="8"/>
       <c r="B157" s="4" t="s">
         <v>4</v>
@@ -22382,7 +22388,7 @@
       </c>
       <c r="V157" s="7"/>
     </row>
-    <row r="158" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A158" s="8"/>
       <c r="B158" s="4" t="s">
         <v>4</v>
@@ -22446,7 +22452,7 @@
       </c>
       <c r="V158" s="7"/>
     </row>
-    <row r="159" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>16</v>
       </c>
@@ -22512,7 +22518,7 @@
       </c>
       <c r="V159" s="7"/>
     </row>
-    <row r="160" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A160" s="8"/>
       <c r="B160" s="4" t="s">
         <v>4</v>
@@ -22576,7 +22582,7 @@
       </c>
       <c r="V160" s="7"/>
     </row>
-    <row r="161" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A161" s="8"/>
       <c r="B161" s="4" t="s">
         <v>4</v>
@@ -22640,7 +22646,7 @@
       </c>
       <c r="V161" s="7"/>
     </row>
-    <row r="162" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A162" s="8"/>
       <c r="B162" s="4" t="s">
         <v>4</v>
@@ -22704,7 +22710,7 @@
       </c>
       <c r="V162" s="7"/>
     </row>
-    <row r="163" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A163" s="8"/>
       <c r="B163" s="4" t="s">
         <v>4</v>
@@ -22768,7 +22774,7 @@
       </c>
       <c r="V163" s="7"/>
     </row>
-    <row r="164" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
       <c r="B164" s="4" t="s">
         <v>4</v>
@@ -22832,7 +22838,7 @@
       </c>
       <c r="V164" s="7"/>
     </row>
-    <row r="165" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A165" s="8"/>
       <c r="B165" s="4" t="s">
         <v>4</v>
@@ -22896,7 +22902,7 @@
       </c>
       <c r="V165" s="7"/>
     </row>
-    <row r="166" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A166" s="8"/>
       <c r="B166" s="4" t="s">
         <v>4</v>
@@ -22960,7 +22966,7 @@
       </c>
       <c r="V166" s="7"/>
     </row>
-    <row r="167" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A167" s="8"/>
       <c r="B167" s="4" t="s">
         <v>4</v>
@@ -23024,7 +23030,7 @@
       </c>
       <c r="V167" s="7"/>
     </row>
-    <row r="168" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
       <c r="B168" s="4" t="s">
         <v>4</v>
@@ -23088,7 +23094,7 @@
       </c>
       <c r="V168" s="7"/>
     </row>
-    <row r="169" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
       <c r="B169" s="4" t="s">
         <v>4</v>
@@ -23152,7 +23158,7 @@
       </c>
       <c r="V169" s="7"/>
     </row>
-    <row r="170" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
       <c r="B170" s="4" t="s">
         <v>4</v>
@@ -23216,7 +23222,7 @@
       </c>
       <c r="V170" s="7"/>
     </row>
-    <row r="171" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A171" s="8"/>
       <c r="B171" s="4" t="s">
         <v>4</v>
@@ -23280,7 +23286,7 @@
       </c>
       <c r="V171" s="7"/>
     </row>
-    <row r="172" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
       <c r="B172" s="4" t="s">
         <v>4</v>
@@ -23344,7 +23350,7 @@
       </c>
       <c r="V172" s="7"/>
     </row>
-    <row r="173" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
       <c r="B173" s="4" t="s">
         <v>4</v>
@@ -23408,7 +23414,7 @@
       </c>
       <c r="V173" s="7"/>
     </row>
-    <row r="174" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A174" s="8"/>
       <c r="B174" s="4" t="s">
         <v>4</v>
@@ -23472,7 +23478,7 @@
       </c>
       <c r="V174" s="7"/>
     </row>
-    <row r="175" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A175" s="8"/>
       <c r="B175" s="4" t="s">
         <v>4</v>
@@ -23536,7 +23542,7 @@
       </c>
       <c r="V175" s="7"/>
     </row>
-    <row r="176" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A176" s="8"/>
       <c r="B176" s="4" t="s">
         <v>4</v>
@@ -23600,7 +23606,7 @@
       </c>
       <c r="V176" s="7"/>
     </row>
-    <row r="177" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A177" s="8"/>
       <c r="B177" s="4" t="s">
         <v>4</v>
@@ -23664,7 +23670,7 @@
       </c>
       <c r="V177" s="7"/>
     </row>
-    <row r="178" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A178" s="8"/>
       <c r="B178" s="4" t="s">
         <v>4</v>
@@ -23728,7 +23734,7 @@
       </c>
       <c r="V178" s="7"/>
     </row>
-    <row r="179" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A179" s="8"/>
       <c r="B179" s="4" t="s">
         <v>4</v>
@@ -23792,7 +23798,7 @@
       </c>
       <c r="V179" s="7"/>
     </row>
-    <row r="180" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A180" s="8"/>
       <c r="B180" s="4" t="s">
         <v>4</v>
@@ -23856,7 +23862,7 @@
       </c>
       <c r="V180" s="7"/>
     </row>
-    <row r="181" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A181" s="8"/>
       <c r="B181" s="4" t="s">
         <v>4</v>
@@ -23920,7 +23926,7 @@
       </c>
       <c r="V181" s="7"/>
     </row>
-    <row r="182" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A182" s="8"/>
       <c r="B182" s="4" t="s">
         <v>4</v>
@@ -23984,7 +23990,7 @@
       </c>
       <c r="V182" s="7"/>
     </row>
-    <row r="183" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A183" s="8"/>
       <c r="B183" s="4" t="s">
         <v>4</v>
@@ -24048,7 +24054,7 @@
       </c>
       <c r="V183" s="7"/>
     </row>
-    <row r="184" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A184" s="8"/>
       <c r="B184" s="4" t="s">
         <v>4</v>
@@ -24112,7 +24118,7 @@
       </c>
       <c r="V184" s="7"/>
     </row>
-    <row r="185" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A185" s="8"/>
       <c r="B185" s="4" t="s">
         <v>4</v>
@@ -24176,7 +24182,7 @@
       </c>
       <c r="V185" s="7"/>
     </row>
-    <row r="186" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A186" s="8"/>
       <c r="B186" s="4" t="s">
         <v>4</v>
@@ -24240,7 +24246,7 @@
       </c>
       <c r="V186" s="7"/>
     </row>
-    <row r="187" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A187" s="3" t="s">
         <v>15</v>
       </c>
@@ -24306,7 +24312,7 @@
       </c>
       <c r="V187" s="7"/>
     </row>
-    <row r="188" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A188" s="8"/>
       <c r="B188" s="4" t="s">
         <v>4</v>
@@ -24370,7 +24376,7 @@
       </c>
       <c r="V188" s="7"/>
     </row>
-    <row r="189" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A189" s="8"/>
       <c r="B189" s="4" t="s">
         <v>4</v>
@@ -24434,7 +24440,7 @@
       </c>
       <c r="V189" s="7"/>
     </row>
-    <row r="190" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A190" s="8"/>
       <c r="B190" s="4" t="s">
         <v>4</v>
@@ -24498,7 +24504,7 @@
       </c>
       <c r="V190" s="7"/>
     </row>
-    <row r="191" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A191" s="8"/>
       <c r="B191" s="4" t="s">
         <v>4</v>
@@ -24562,7 +24568,7 @@
       </c>
       <c r="V191" s="7"/>
     </row>
-    <row r="192" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A192" s="8"/>
       <c r="B192" s="4" t="s">
         <v>4</v>
@@ -24626,7 +24632,7 @@
       </c>
       <c r="V192" s="7"/>
     </row>
-    <row r="193" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A193" s="8"/>
       <c r="B193" s="4" t="s">
         <v>4</v>
@@ -24690,7 +24696,7 @@
       </c>
       <c r="V193" s="7"/>
     </row>
-    <row r="194" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A194" s="8"/>
       <c r="B194" s="4" t="s">
         <v>4</v>
@@ -24754,7 +24760,7 @@
       </c>
       <c r="V194" s="7"/>
     </row>
-    <row r="195" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A195" s="8"/>
       <c r="B195" s="4" t="s">
         <v>4</v>
@@ -24818,7 +24824,7 @@
       </c>
       <c r="V195" s="7"/>
     </row>
-    <row r="196" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A196" s="8"/>
       <c r="B196" s="4" t="s">
         <v>4</v>
@@ -24882,7 +24888,7 @@
       </c>
       <c r="V196" s="7"/>
     </row>
-    <row r="197" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A197" s="8"/>
       <c r="B197" s="4" t="s">
         <v>4</v>
@@ -24946,7 +24952,7 @@
       </c>
       <c r="V197" s="7"/>
     </row>
-    <row r="198" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A198" s="8"/>
       <c r="B198" s="4" t="s">
         <v>4</v>
@@ -25010,7 +25016,7 @@
       </c>
       <c r="V198" s="7"/>
     </row>
-    <row r="199" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A199" s="8"/>
       <c r="B199" s="4" t="s">
         <v>4</v>
@@ -25074,7 +25080,7 @@
       </c>
       <c r="V199" s="7"/>
     </row>
-    <row r="200" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A200" s="8"/>
       <c r="B200" s="4" t="s">
         <v>4</v>
@@ -25138,7 +25144,7 @@
       </c>
       <c r="V200" s="7"/>
     </row>
-    <row r="201" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A201" s="8"/>
       <c r="B201" s="4" t="s">
         <v>4</v>
@@ -25202,7 +25208,7 @@
       </c>
       <c r="V201" s="7"/>
     </row>
-    <row r="202" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A202" s="8"/>
       <c r="B202" s="4" t="s">
         <v>4</v>
@@ -25266,7 +25272,7 @@
       </c>
       <c r="V202" s="7"/>
     </row>
-    <row r="203" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A203" s="3" t="s">
         <v>14</v>
       </c>
@@ -25332,7 +25338,7 @@
       </c>
       <c r="V203" s="7"/>
     </row>
-    <row r="204" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A204" s="8"/>
       <c r="B204" s="4" t="s">
         <v>4</v>
@@ -25396,7 +25402,7 @@
       </c>
       <c r="V204" s="7"/>
     </row>
-    <row r="205" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A205" s="8"/>
       <c r="B205" s="4" t="s">
         <v>4</v>
@@ -25460,7 +25466,7 @@
       </c>
       <c r="V205" s="7"/>
     </row>
-    <row r="206" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A206" s="8"/>
       <c r="B206" s="4" t="s">
         <v>4</v>
@@ -25524,7 +25530,7 @@
       </c>
       <c r="V206" s="7"/>
     </row>
-    <row r="207" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A207" s="8"/>
       <c r="B207" s="4" t="s">
         <v>4</v>
@@ -25588,7 +25594,7 @@
       </c>
       <c r="V207" s="7"/>
     </row>
-    <row r="208" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A208" s="8"/>
       <c r="B208" s="4" t="s">
         <v>4</v>
@@ -25652,7 +25658,7 @@
       </c>
       <c r="V208" s="7"/>
     </row>
-    <row r="209" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A209" s="8"/>
       <c r="B209" s="4" t="s">
         <v>4</v>
@@ -25716,7 +25722,7 @@
       </c>
       <c r="V209" s="7"/>
     </row>
-    <row r="210" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A210" s="8"/>
       <c r="B210" s="4" t="s">
         <v>4</v>
@@ -25780,7 +25786,7 @@
       </c>
       <c r="V210" s="7"/>
     </row>
-    <row r="211" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A211" s="8"/>
       <c r="B211" s="4" t="s">
         <v>4</v>
@@ -25844,7 +25850,7 @@
       </c>
       <c r="V211" s="7"/>
     </row>
-    <row r="212" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A212" s="8"/>
       <c r="B212" s="4" t="s">
         <v>4</v>
@@ -25908,7 +25914,7 @@
       </c>
       <c r="V212" s="7"/>
     </row>
-    <row r="213" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A213" s="8"/>
       <c r="B213" s="4" t="s">
         <v>4</v>
@@ -25972,7 +25978,7 @@
       </c>
       <c r="V213" s="7"/>
     </row>
-    <row r="214" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A214" s="8"/>
       <c r="B214" s="4" t="s">
         <v>4</v>
@@ -26036,7 +26042,7 @@
       </c>
       <c r="V214" s="7"/>
     </row>
-    <row r="215" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A215" s="8"/>
       <c r="B215" s="4" t="s">
         <v>4</v>
@@ -26100,7 +26106,7 @@
       </c>
       <c r="V215" s="7"/>
     </row>
-    <row r="216" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A216" s="3" t="s">
         <v>13</v>
       </c>
@@ -26166,7 +26172,7 @@
       </c>
       <c r="V216" s="7"/>
     </row>
-    <row r="217" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A217" s="8"/>
       <c r="B217" s="4" t="s">
         <v>4</v>
@@ -26230,7 +26236,7 @@
       </c>
       <c r="V217" s="7"/>
     </row>
-    <row r="218" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A218" s="8"/>
       <c r="B218" s="4" t="s">
         <v>4</v>
@@ -26294,7 +26300,7 @@
       </c>
       <c r="V218" s="7"/>
     </row>
-    <row r="219" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A219" s="8"/>
       <c r="B219" s="4" t="s">
         <v>4</v>
@@ -26358,7 +26364,7 @@
       </c>
       <c r="V219" s="7"/>
     </row>
-    <row r="220" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A220" s="8"/>
       <c r="B220" s="4" t="s">
         <v>4</v>
@@ -26422,7 +26428,7 @@
       </c>
       <c r="V220" s="7"/>
     </row>
-    <row r="221" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A221" s="8"/>
       <c r="B221" s="4" t="s">
         <v>4</v>
@@ -26486,7 +26492,7 @@
       </c>
       <c r="V221" s="7"/>
     </row>
-    <row r="222" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A222" s="8"/>
       <c r="B222" s="4" t="s">
         <v>4</v>
@@ -26550,7 +26556,7 @@
       </c>
       <c r="V222" s="7"/>
     </row>
-    <row r="223" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A223" s="8"/>
       <c r="B223" s="4" t="s">
         <v>4</v>
@@ -26614,7 +26620,7 @@
       </c>
       <c r="V223" s="7"/>
     </row>
-    <row r="224" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A224" s="8"/>
       <c r="B224" s="4" t="s">
         <v>4</v>
@@ -26678,7 +26684,7 @@
       </c>
       <c r="V224" s="7"/>
     </row>
-    <row r="225" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A225" s="8"/>
       <c r="B225" s="4" t="s">
         <v>4</v>
@@ -26742,7 +26748,7 @@
       </c>
       <c r="V225" s="7"/>
     </row>
-    <row r="226" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A226" s="8"/>
       <c r="B226" s="4" t="s">
         <v>4</v>
@@ -26806,7 +26812,7 @@
       </c>
       <c r="V226" s="7"/>
     </row>
-    <row r="227" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A227" s="8"/>
       <c r="B227" s="4" t="s">
         <v>4</v>
@@ -26870,7 +26876,7 @@
       </c>
       <c r="V227" s="7"/>
     </row>
-    <row r="228" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A228" s="8"/>
       <c r="B228" s="4" t="s">
         <v>4</v>
@@ -26934,7 +26940,7 @@
       </c>
       <c r="V228" s="7"/>
     </row>
-    <row r="229" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A229" s="8"/>
       <c r="B229" s="4" t="s">
         <v>4</v>
@@ -26998,7 +27004,7 @@
       </c>
       <c r="V229" s="7"/>
     </row>
-    <row r="230" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A230" s="8"/>
       <c r="B230" s="4" t="s">
         <v>4</v>
@@ -27062,7 +27068,7 @@
       </c>
       <c r="V230" s="7"/>
     </row>
-    <row r="231" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A231" s="8"/>
       <c r="B231" s="4" t="s">
         <v>4</v>
@@ -27126,7 +27132,7 @@
       </c>
       <c r="V231" s="7"/>
     </row>
-    <row r="232" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A232" s="8"/>
       <c r="B232" s="4" t="s">
         <v>4</v>
@@ -27190,7 +27196,7 @@
       </c>
       <c r="V232" s="7"/>
     </row>
-    <row r="233" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A233" s="8"/>
       <c r="B233" s="4" t="s">
         <v>4</v>
@@ -27254,7 +27260,7 @@
       </c>
       <c r="V233" s="7"/>
     </row>
-    <row r="234" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A234" s="8"/>
       <c r="B234" s="4" t="s">
         <v>4</v>
@@ -27318,7 +27324,7 @@
       </c>
       <c r="V234" s="7"/>
     </row>
-    <row r="235" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A235" s="8"/>
       <c r="B235" s="4" t="s">
         <v>4</v>
@@ -27382,7 +27388,7 @@
       </c>
       <c r="V235" s="7"/>
     </row>
-    <row r="236" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A236" s="8"/>
       <c r="B236" s="4" t="s">
         <v>4</v>
@@ -27446,7 +27452,7 @@
       </c>
       <c r="V236" s="7"/>
     </row>
-    <row r="237" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A237" s="3" t="s">
         <v>12</v>
       </c>
@@ -27512,7 +27518,7 @@
       </c>
       <c r="V237" s="7"/>
     </row>
-    <row r="238" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A238" s="8"/>
       <c r="B238" s="4" t="s">
         <v>4</v>
@@ -27576,7 +27582,7 @@
       </c>
       <c r="V238" s="7"/>
     </row>
-    <row r="239" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A239" s="8"/>
       <c r="B239" s="4" t="s">
         <v>4</v>
@@ -27640,7 +27646,7 @@
       </c>
       <c r="V239" s="7"/>
     </row>
-    <row r="240" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A240" s="8"/>
       <c r="B240" s="4" t="s">
         <v>4</v>
@@ -27704,7 +27710,7 @@
       </c>
       <c r="V240" s="7"/>
     </row>
-    <row r="241" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A241" s="8"/>
       <c r="B241" s="4" t="s">
         <v>4</v>
@@ -27768,7 +27774,7 @@
       </c>
       <c r="V241" s="7"/>
     </row>
-    <row r="242" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A242" s="8"/>
       <c r="B242" s="4" t="s">
         <v>4</v>
@@ -27832,7 +27838,7 @@
       </c>
       <c r="V242" s="7"/>
     </row>
-    <row r="243" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A243" s="8"/>
       <c r="B243" s="4" t="s">
         <v>4</v>
@@ -27896,7 +27902,7 @@
       </c>
       <c r="V243" s="7"/>
     </row>
-    <row r="244" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A244" s="8"/>
       <c r="B244" s="4" t="s">
         <v>4</v>
@@ -27960,7 +27966,7 @@
       </c>
       <c r="V244" s="7"/>
     </row>
-    <row r="245" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A245" s="8"/>
       <c r="B245" s="4" t="s">
         <v>4</v>
@@ -28024,7 +28030,7 @@
       </c>
       <c r="V245" s="7"/>
     </row>
-    <row r="246" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A246" s="8"/>
       <c r="B246" s="4" t="s">
         <v>4</v>
@@ -28088,7 +28094,7 @@
       </c>
       <c r="V246" s="7"/>
     </row>
-    <row r="247" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A247" s="8"/>
       <c r="B247" s="4" t="s">
         <v>4</v>
@@ -28152,7 +28158,7 @@
       </c>
       <c r="V247" s="7"/>
     </row>
-    <row r="248" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A248" s="8"/>
       <c r="B248" s="4" t="s">
         <v>4</v>
@@ -28216,7 +28222,7 @@
       </c>
       <c r="V248" s="7"/>
     </row>
-    <row r="249" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A249" s="8"/>
       <c r="B249" s="4" t="s">
         <v>4</v>
@@ -28280,7 +28286,7 @@
       </c>
       <c r="V249" s="7"/>
     </row>
-    <row r="250" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A250" s="9"/>
       <c r="B250" s="4" t="s">
         <v>4</v>
@@ -28344,7 +28350,7 @@
       </c>
       <c r="V250" s="7"/>
     </row>
-    <row r="251" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A251" s="8"/>
       <c r="B251" s="4" t="s">
         <v>4</v>
@@ -28408,7 +28414,7 @@
       </c>
       <c r="V251" s="7"/>
     </row>
-    <row r="252" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A252" s="8"/>
       <c r="B252" s="4" t="s">
         <v>4</v>
@@ -28472,7 +28478,7 @@
       </c>
       <c r="V252" s="7"/>
     </row>
-    <row r="253" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A253" s="8"/>
       <c r="B253" s="4" t="s">
         <v>4</v>
@@ -28536,7 +28542,7 @@
       </c>
       <c r="V253" s="7"/>
     </row>
-    <row r="254" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A254" s="8"/>
       <c r="B254" s="4" t="s">
         <v>4</v>
@@ -28600,7 +28606,7 @@
       </c>
       <c r="V254" s="7"/>
     </row>
-    <row r="255" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A255" s="8"/>
       <c r="B255" s="4" t="s">
         <v>4</v>
@@ -28664,7 +28670,7 @@
       </c>
       <c r="V255" s="7"/>
     </row>
-    <row r="256" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A256" s="8"/>
       <c r="B256" s="4" t="s">
         <v>4</v>
@@ -28728,7 +28734,7 @@
       </c>
       <c r="V256" s="7"/>
     </row>
-    <row r="257" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A257" s="8"/>
       <c r="B257" s="4" t="s">
         <v>4</v>
@@ -28792,7 +28798,7 @@
       </c>
       <c r="V257" s="7"/>
     </row>
-    <row r="258" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A258" s="8"/>
       <c r="B258" s="4" t="s">
         <v>4</v>
@@ -28856,7 +28862,7 @@
       </c>
       <c r="V258" s="7"/>
     </row>
-    <row r="259" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A259" s="8"/>
       <c r="B259" s="4" t="s">
         <v>4</v>
@@ -28920,7 +28926,7 @@
       </c>
       <c r="V259" s="7"/>
     </row>
-    <row r="260" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A260" s="8"/>
       <c r="B260" s="4" t="s">
         <v>4</v>
@@ -28984,7 +28990,7 @@
       </c>
       <c r="V260" s="7"/>
     </row>
-    <row r="261" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A261" s="8"/>
       <c r="B261" s="4" t="s">
         <v>4</v>
@@ -29048,7 +29054,7 @@
       </c>
       <c r="V261" s="7"/>
     </row>
-    <row r="262" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A262" s="8"/>
       <c r="B262" s="4" t="s">
         <v>4</v>
@@ -29112,7 +29118,7 @@
       </c>
       <c r="V262" s="7"/>
     </row>
-    <row r="263" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A263" s="8"/>
       <c r="B263" s="4" t="s">
         <v>4</v>
@@ -29176,7 +29182,7 @@
       </c>
       <c r="V263" s="7"/>
     </row>
-    <row r="264" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A264" s="8"/>
       <c r="B264" s="4" t="s">
         <v>4</v>
@@ -29240,7 +29246,7 @@
       </c>
       <c r="V264" s="7"/>
     </row>
-    <row r="265" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A265" s="8"/>
       <c r="B265" s="4" t="s">
         <v>4</v>
@@ -29304,7 +29310,7 @@
       </c>
       <c r="V265" s="7"/>
     </row>
-    <row r="266" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A266" s="8"/>
       <c r="B266" s="4" t="s">
         <v>4</v>
@@ -29368,7 +29374,7 @@
       </c>
       <c r="V266" s="7"/>
     </row>
-    <row r="267" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A267" s="8"/>
       <c r="B267" s="4" t="s">
         <v>4</v>
@@ -29432,7 +29438,7 @@
       </c>
       <c r="V267" s="7"/>
     </row>
-    <row r="268" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A268" s="8"/>
       <c r="B268" s="4" t="s">
         <v>4</v>
@@ -29496,7 +29502,7 @@
       </c>
       <c r="V268" s="7"/>
     </row>
-    <row r="269" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A269" s="8"/>
       <c r="B269" s="4" t="s">
         <v>4</v>
@@ -29560,7 +29566,7 @@
       </c>
       <c r="V269" s="7"/>
     </row>
-    <row r="270" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A270" s="8"/>
       <c r="B270" s="4" t="s">
         <v>4</v>
@@ -29624,7 +29630,7 @@
       </c>
       <c r="V270" s="7"/>
     </row>
-    <row r="271" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A271" s="8"/>
       <c r="B271" s="4" t="s">
         <v>4</v>
@@ -29688,7 +29694,7 @@
       </c>
       <c r="V271" s="7"/>
     </row>
-    <row r="272" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A272" s="9"/>
       <c r="B272" s="4" t="s">
         <v>4</v>
@@ -29752,7 +29758,7 @@
       </c>
       <c r="V272" s="7"/>
     </row>
-    <row r="273" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A273" s="8"/>
       <c r="B273" s="4" t="s">
         <v>4</v>
@@ -29816,7 +29822,7 @@
       </c>
       <c r="V273" s="7"/>
     </row>
-    <row r="274" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A274" s="8"/>
       <c r="B274" s="4" t="s">
         <v>4</v>
@@ -29880,7 +29886,7 @@
       </c>
       <c r="V274" s="7"/>
     </row>
-    <row r="275" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A275" s="8"/>
       <c r="B275" s="4" t="s">
         <v>4</v>
@@ -29944,7 +29950,7 @@
       </c>
       <c r="V275" s="7"/>
     </row>
-    <row r="276" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A276" s="8"/>
       <c r="B276" s="4" t="s">
         <v>4</v>
@@ -30008,7 +30014,7 @@
       </c>
       <c r="V276" s="7"/>
     </row>
-    <row r="277" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A277" s="8"/>
       <c r="B277" s="4" t="s">
         <v>4</v>
@@ -30072,7 +30078,7 @@
       </c>
       <c r="V277" s="7"/>
     </row>
-    <row r="278" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A278" s="8"/>
       <c r="B278" s="4" t="s">
         <v>4</v>
@@ -30136,7 +30142,7 @@
       </c>
       <c r="V278" s="7"/>
     </row>
-    <row r="279" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A279" s="8"/>
       <c r="B279" s="4" t="s">
         <v>4</v>
@@ -30200,7 +30206,7 @@
       </c>
       <c r="V279" s="7"/>
     </row>
-    <row r="280" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A280" s="8"/>
       <c r="B280" s="4" t="s">
         <v>4</v>
@@ -30264,7 +30270,7 @@
       </c>
       <c r="V280" s="7"/>
     </row>
-    <row r="281" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A281" s="8"/>
       <c r="B281" s="4" t="s">
         <v>4</v>
@@ -30328,7 +30334,7 @@
       </c>
       <c r="V281" s="7"/>
     </row>
-    <row r="282" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A282" s="8"/>
       <c r="B282" s="4" t="s">
         <v>4</v>
@@ -30392,7 +30398,7 @@
       </c>
       <c r="V282" s="7"/>
     </row>
-    <row r="283" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A283" s="8"/>
       <c r="B283" s="4" t="s">
         <v>4</v>
@@ -30456,7 +30462,7 @@
       </c>
       <c r="V283" s="7"/>
     </row>
-    <row r="284" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A284" s="8"/>
       <c r="B284" s="4" t="s">
         <v>4</v>
@@ -30520,7 +30526,7 @@
       </c>
       <c r="V284" s="7"/>
     </row>
-    <row r="285" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A285" s="8"/>
       <c r="B285" s="4" t="s">
         <v>4</v>
@@ -30584,7 +30590,7 @@
       </c>
       <c r="V285" s="7"/>
     </row>
-    <row r="286" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A286" s="8"/>
       <c r="B286" s="4" t="s">
         <v>4</v>
@@ -30648,7 +30654,7 @@
       </c>
       <c r="V286" s="7"/>
     </row>
-    <row r="287" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A287" s="8"/>
       <c r="B287" s="4" t="s">
         <v>4</v>
@@ -30712,7 +30718,7 @@
       </c>
       <c r="V287" s="7"/>
     </row>
-    <row r="288" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A288" s="8"/>
       <c r="B288" s="4" t="s">
         <v>4</v>
@@ -30776,7 +30782,7 @@
       </c>
       <c r="V288" s="7"/>
     </row>
-    <row r="289" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A289" s="3" t="s">
         <v>10</v>
       </c>
@@ -30842,7 +30848,7 @@
       </c>
       <c r="V289" s="7"/>
     </row>
-    <row r="290" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A290" s="8"/>
       <c r="B290" s="4" t="s">
         <v>4</v>
@@ -30906,7 +30912,7 @@
       </c>
       <c r="V290" s="7"/>
     </row>
-    <row r="291" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A291" s="8"/>
       <c r="B291" s="4" t="s">
         <v>4</v>
@@ -30970,7 +30976,7 @@
       </c>
       <c r="V291" s="7"/>
     </row>
-    <row r="292" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A292" s="8"/>
       <c r="B292" s="4" t="s">
         <v>4</v>
@@ -31034,7 +31040,7 @@
       </c>
       <c r="V292" s="7"/>
     </row>
-    <row r="293" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A293" s="8"/>
       <c r="B293" s="4" t="s">
         <v>4</v>
@@ -31098,7 +31104,7 @@
       </c>
       <c r="V293" s="7"/>
     </row>
-    <row r="294" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A294" s="8"/>
       <c r="B294" s="4" t="s">
         <v>4</v>
@@ -31162,7 +31168,7 @@
       </c>
       <c r="V294" s="7"/>
     </row>
-    <row r="295" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A295" s="8"/>
       <c r="B295" s="4" t="s">
         <v>4</v>
@@ -31226,7 +31232,7 @@
       </c>
       <c r="V295" s="7"/>
     </row>
-    <row r="296" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A296" s="8"/>
       <c r="B296" s="4" t="s">
         <v>4</v>
@@ -31290,7 +31296,7 @@
       </c>
       <c r="V296" s="7"/>
     </row>
-    <row r="297" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A297" s="8"/>
       <c r="B297" s="4" t="s">
         <v>4</v>
@@ -31354,7 +31360,7 @@
       </c>
       <c r="V297" s="7"/>
     </row>
-    <row r="298" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A298" s="8"/>
       <c r="B298" s="4" t="s">
         <v>4</v>
@@ -31418,7 +31424,7 @@
       </c>
       <c r="V298" s="7"/>
     </row>
-    <row r="299" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A299" s="8"/>
       <c r="B299" s="4" t="s">
         <v>4</v>
@@ -31482,7 +31488,7 @@
       </c>
       <c r="V299" s="7"/>
     </row>
-    <row r="300" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A300" s="8"/>
       <c r="B300" s="4" t="s">
         <v>4</v>
@@ -31546,7 +31552,7 @@
       </c>
       <c r="V300" s="7"/>
     </row>
-    <row r="301" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A301" s="8"/>
       <c r="B301" s="4" t="s">
         <v>4</v>
@@ -31610,7 +31616,7 @@
       </c>
       <c r="V301" s="7"/>
     </row>
-    <row r="302" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A302" s="8"/>
       <c r="B302" s="4" t="s">
         <v>4</v>
@@ -31674,7 +31680,7 @@
       </c>
       <c r="V302" s="7"/>
     </row>
-    <row r="303" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A303" s="8"/>
       <c r="B303" s="4" t="s">
         <v>4</v>
@@ -31738,7 +31744,7 @@
       </c>
       <c r="V303" s="7"/>
     </row>
-    <row r="304" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A304" s="8"/>
       <c r="B304" s="4" t="s">
         <v>4</v>
@@ -31802,7 +31808,7 @@
       </c>
       <c r="V304" s="7"/>
     </row>
-    <row r="305" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A305" s="8"/>
       <c r="B305" s="4" t="s">
         <v>4</v>
@@ -31866,7 +31872,7 @@
       </c>
       <c r="V305" s="7"/>
     </row>
-    <row r="306" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A306" s="8"/>
       <c r="B306" s="4" t="s">
         <v>4</v>
@@ -31930,7 +31936,7 @@
       </c>
       <c r="V306" s="7"/>
     </row>
-    <row r="307" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A307" s="8"/>
       <c r="B307" s="4" t="s">
         <v>4</v>
@@ -31994,7 +32000,7 @@
       </c>
       <c r="V307" s="7"/>
     </row>
-    <row r="308" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A308" s="8"/>
       <c r="B308" s="4" t="s">
         <v>4</v>
@@ -32058,7 +32064,7 @@
       </c>
       <c r="V308" s="7"/>
     </row>
-    <row r="309" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A309" s="8"/>
       <c r="B309" s="4" t="s">
         <v>4</v>
@@ -32122,7 +32128,7 @@
       </c>
       <c r="V309" s="7"/>
     </row>
-    <row r="310" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A310" s="8"/>
       <c r="B310" s="4" t="s">
         <v>4</v>
@@ -32186,7 +32192,7 @@
       </c>
       <c r="V310" s="7"/>
     </row>
-    <row r="311" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A311" s="8"/>
       <c r="B311" s="4" t="s">
         <v>4</v>
@@ -32250,7 +32256,7 @@
       </c>
       <c r="V311" s="7"/>
     </row>
-    <row r="312" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A312" s="8"/>
       <c r="B312" s="4" t="s">
         <v>4</v>
@@ -32314,7 +32320,7 @@
       </c>
       <c r="V312" s="7"/>
     </row>
-    <row r="313" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A313" s="8"/>
       <c r="B313" s="4" t="s">
         <v>4</v>
@@ -32378,7 +32384,7 @@
       </c>
       <c r="V313" s="7"/>
     </row>
-    <row r="314" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A314" s="8"/>
       <c r="B314" s="4" t="s">
         <v>4</v>
@@ -32442,7 +32448,7 @@
       </c>
       <c r="V314" s="7"/>
     </row>
-    <row r="315" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A315" s="8"/>
       <c r="B315" s="4" t="s">
         <v>4</v>
@@ -32506,7 +32512,7 @@
       </c>
       <c r="V315" s="7"/>
     </row>
-    <row r="316" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A316" s="8"/>
       <c r="B316" s="4" t="s">
         <v>4</v>
@@ -32570,7 +32576,7 @@
       </c>
       <c r="V316" s="7"/>
     </row>
-    <row r="317" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A317" s="8"/>
       <c r="B317" s="4" t="s">
         <v>4</v>
@@ -32634,7 +32640,7 @@
       </c>
       <c r="V317" s="7"/>
     </row>
-    <row r="318" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A318" s="8"/>
       <c r="B318" s="4" t="s">
         <v>4</v>
@@ -32698,7 +32704,7 @@
       </c>
       <c r="V318" s="7"/>
     </row>
-    <row r="319" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A319" s="8"/>
       <c r="B319" s="4" t="s">
         <v>4</v>
@@ -32762,7 +32768,7 @@
       </c>
       <c r="V319" s="7"/>
     </row>
-    <row r="320" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A320" s="8"/>
       <c r="B320" s="4" t="s">
         <v>4</v>
@@ -32826,7 +32832,7 @@
       </c>
       <c r="V320" s="7"/>
     </row>
-    <row r="321" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A321" s="8"/>
       <c r="B321" s="4" t="s">
         <v>4</v>
@@ -32890,7 +32896,7 @@
       </c>
       <c r="V321" s="7"/>
     </row>
-    <row r="322" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A322" s="9"/>
       <c r="B322" s="4" t="s">
         <v>4</v>
@@ -32954,7 +32960,7 @@
       </c>
       <c r="V322" s="7"/>
     </row>
-    <row r="323" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A323" s="8"/>
       <c r="B323" s="4" t="s">
         <v>4</v>
@@ -33018,7 +33024,7 @@
       </c>
       <c r="V323" s="7"/>
     </row>
-    <row r="324" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A324" s="8"/>
       <c r="B324" s="4" t="s">
         <v>4</v>
@@ -33082,7 +33088,7 @@
       </c>
       <c r="V324" s="7"/>
     </row>
-    <row r="325" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A325" s="8"/>
       <c r="B325" s="4" t="s">
         <v>4</v>
@@ -33146,7 +33152,7 @@
       </c>
       <c r="V325" s="7"/>
     </row>
-    <row r="326" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A326" s="8"/>
       <c r="B326" s="4" t="s">
         <v>4</v>
@@ -33210,7 +33216,7 @@
       </c>
       <c r="V326" s="7"/>
     </row>
-    <row r="327" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A327" s="8"/>
       <c r="B327" s="4" t="s">
         <v>4</v>
@@ -33274,7 +33280,7 @@
       </c>
       <c r="V327" s="7"/>
     </row>
-    <row r="328" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A328" s="8"/>
       <c r="B328" s="4" t="s">
         <v>4</v>
@@ -33338,7 +33344,7 @@
       </c>
       <c r="V328" s="7"/>
     </row>
-    <row r="329" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A329" s="8"/>
       <c r="B329" s="4" t="s">
         <v>4</v>
@@ -33402,7 +33408,7 @@
       </c>
       <c r="V329" s="7"/>
     </row>
-    <row r="330" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A330" s="8"/>
       <c r="B330" s="4" t="s">
         <v>4</v>
@@ -33466,7 +33472,7 @@
       </c>
       <c r="V330" s="7"/>
     </row>
-    <row r="331" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A331" s="8"/>
       <c r="B331" s="4" t="s">
         <v>4</v>
@@ -33530,7 +33536,7 @@
       </c>
       <c r="V331" s="7"/>
     </row>
-    <row r="332" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A332" s="8"/>
       <c r="B332" s="4" t="s">
         <v>4</v>
@@ -33594,7 +33600,7 @@
       </c>
       <c r="V332" s="7"/>
     </row>
-    <row r="333" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A333" s="8"/>
       <c r="B333" s="4" t="s">
         <v>4</v>
@@ -33658,7 +33664,7 @@
       </c>
       <c r="V333" s="7"/>
     </row>
-    <row r="334" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A334" s="8"/>
       <c r="B334" s="4" t="s">
         <v>4</v>
@@ -33722,7 +33728,7 @@
       </c>
       <c r="V334" s="7"/>
     </row>
-    <row r="335" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A335" s="8"/>
       <c r="B335" s="4" t="s">
         <v>4</v>
@@ -33786,7 +33792,7 @@
       </c>
       <c r="V335" s="7"/>
     </row>
-    <row r="336" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A336" s="3" t="s">
         <v>22</v>
       </c>
@@ -33852,7 +33858,7 @@
       </c>
       <c r="V336" s="7"/>
     </row>
-    <row r="337" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A337" s="8"/>
       <c r="B337" s="4" t="s">
         <v>4</v>
@@ -33916,7 +33922,7 @@
       </c>
       <c r="V337" s="7"/>
     </row>
-    <row r="338" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A338" s="8"/>
       <c r="B338" s="4" t="s">
         <v>4</v>
@@ -33980,7 +33986,7 @@
       </c>
       <c r="V338" s="7"/>
     </row>
-    <row r="339" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A339" s="8"/>
       <c r="B339" s="4" t="s">
         <v>4</v>
@@ -34044,7 +34050,7 @@
       </c>
       <c r="V339" s="7"/>
     </row>
-    <row r="340" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A340" s="8"/>
       <c r="B340" s="4" t="s">
         <v>4</v>
@@ -34108,7 +34114,7 @@
       </c>
       <c r="V340" s="7"/>
     </row>
-    <row r="341" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A341" s="8"/>
       <c r="B341" s="4" t="s">
         <v>4</v>
@@ -34170,7 +34176,7 @@
       </c>
       <c r="V341" s="7"/>
     </row>
-    <row r="342" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A342" s="8"/>
       <c r="B342" s="4" t="s">
         <v>4</v>
@@ -34234,7 +34240,7 @@
       </c>
       <c r="V342" s="7"/>
     </row>
-    <row r="343" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A343" s="8"/>
       <c r="B343" s="4" t="s">
         <v>4</v>
@@ -34298,7 +34304,7 @@
       </c>
       <c r="V343" s="7"/>
     </row>
-    <row r="344" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A344" s="9"/>
       <c r="B344" s="4" t="s">
         <v>4</v>
@@ -34362,7 +34368,7 @@
       </c>
       <c r="V344" s="7"/>
     </row>
-    <row r="345" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A345" s="8"/>
       <c r="B345" s="4" t="s">
         <v>4</v>
@@ -34426,7 +34432,7 @@
       </c>
       <c r="V345" s="7"/>
     </row>
-    <row r="346" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A346" s="8"/>
       <c r="B346" s="4" t="s">
         <v>4</v>
@@ -34490,7 +34496,7 @@
       </c>
       <c r="V346" s="7"/>
     </row>
-    <row r="347" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A347" s="8"/>
       <c r="B347" s="4" t="s">
         <v>4</v>
@@ -34554,7 +34560,7 @@
       </c>
       <c r="V347" s="7"/>
     </row>
-    <row r="348" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A348" s="8"/>
       <c r="B348" s="4" t="s">
         <v>4</v>
@@ -34618,7 +34624,7 @@
       </c>
       <c r="V348" s="7"/>
     </row>
-    <row r="349" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A349" s="8"/>
       <c r="B349" s="4" t="s">
         <v>4</v>
@@ -34682,7 +34688,7 @@
       </c>
       <c r="V349" s="7"/>
     </row>
-    <row r="350" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A350" s="8"/>
       <c r="B350" s="4" t="s">
         <v>4</v>
@@ -34746,7 +34752,7 @@
       </c>
       <c r="V350" s="7"/>
     </row>
-    <row r="351" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A351" s="8"/>
       <c r="B351" s="4" t="s">
         <v>4</v>
@@ -34810,7 +34816,7 @@
       </c>
       <c r="V351" s="7"/>
     </row>
-    <row r="352" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A352" s="8"/>
       <c r="B352" s="4" t="s">
         <v>4</v>
@@ -34874,7 +34880,7 @@
       </c>
       <c r="V352" s="7"/>
     </row>
-    <row r="353" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A353" s="8"/>
       <c r="B353" s="4" t="s">
         <v>4</v>
@@ -34938,7 +34944,7 @@
       </c>
       <c r="V353" s="7"/>
     </row>
-    <row r="354" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A354" s="8"/>
       <c r="B354" s="4" t="s">
         <v>4</v>
@@ -35002,7 +35008,7 @@
       </c>
       <c r="V354" s="7"/>
     </row>
-    <row r="355" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A355" s="8"/>
       <c r="B355" s="4" t="s">
         <v>4</v>
@@ -35066,7 +35072,7 @@
       </c>
       <c r="V355" s="7"/>
     </row>
-    <row r="356" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A356" s="8"/>
       <c r="B356" s="4" t="s">
         <v>4</v>
@@ -35130,7 +35136,7 @@
       </c>
       <c r="V356" s="7"/>
     </row>
-    <row r="357" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A357" s="8"/>
       <c r="B357" s="4" t="s">
         <v>4</v>
@@ -35194,7 +35200,7 @@
       </c>
       <c r="V357" s="7"/>
     </row>
-    <row r="358" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A358" s="8"/>
       <c r="B358" s="4" t="s">
         <v>4</v>
@@ -35258,7 +35264,7 @@
       </c>
       <c r="V358" s="7"/>
     </row>
-    <row r="359" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A359" s="8"/>
       <c r="B359" s="4" t="s">
         <v>4</v>
@@ -35322,7 +35328,7 @@
       </c>
       <c r="V359" s="7"/>
     </row>
-    <row r="360" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A360" s="8"/>
       <c r="B360" s="4" t="s">
         <v>4</v>
@@ -35386,7 +35392,7 @@
       </c>
       <c r="V360" s="7"/>
     </row>
-    <row r="361" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A361" s="8"/>
       <c r="B361" s="4" t="s">
         <v>4</v>
@@ -35450,7 +35456,7 @@
       </c>
       <c r="V361" s="7"/>
     </row>
-    <row r="362" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A362" s="8"/>
       <c r="B362" s="4" t="s">
         <v>4</v>
@@ -35514,7 +35520,7 @@
       </c>
       <c r="V362" s="7"/>
     </row>
-    <row r="363" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A363" s="8"/>
       <c r="B363" s="4" t="s">
         <v>4</v>
@@ -35578,7 +35584,7 @@
       </c>
       <c r="V363" s="7"/>
     </row>
-    <row r="364" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A364" s="8"/>
       <c r="B364" s="4" t="s">
         <v>4</v>
@@ -35642,7 +35648,7 @@
       </c>
       <c r="V364" s="7"/>
     </row>
-    <row r="365" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A365" s="8"/>
       <c r="B365" s="4" t="s">
         <v>4</v>
@@ -35706,7 +35712,7 @@
       </c>
       <c r="V365" s="7"/>
     </row>
-    <row r="366" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A366" s="8"/>
       <c r="B366" s="4" t="s">
         <v>4</v>
@@ -35770,7 +35776,7 @@
       </c>
       <c r="V366" s="7"/>
     </row>
-    <row r="367" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A367" s="8"/>
       <c r="B367" s="4" t="s">
         <v>4</v>
@@ -35832,7 +35838,7 @@
       </c>
       <c r="V367" s="7"/>
     </row>
-    <row r="368" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A368" s="8"/>
       <c r="B368" s="4" t="s">
         <v>4</v>
@@ -35894,7 +35900,7 @@
       </c>
       <c r="V368" s="7"/>
     </row>
-    <row r="369" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A369" s="8"/>
       <c r="B369" s="4" t="s">
         <v>4</v>
@@ -35956,7 +35962,7 @@
       </c>
       <c r="V369" s="7"/>
     </row>
-    <row r="370" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A370" s="8"/>
       <c r="B370" s="4" t="s">
         <v>4</v>
@@ -36020,7 +36026,7 @@
       </c>
       <c r="V370" s="7"/>
     </row>
-    <row r="371" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A371" s="8"/>
       <c r="B371" s="4" t="s">
         <v>4</v>
@@ -36084,7 +36090,7 @@
       </c>
       <c r="V371" s="7"/>
     </row>
-    <row r="372" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A372" s="8"/>
       <c r="B372" s="4" t="s">
         <v>4</v>
@@ -36148,7 +36154,7 @@
       </c>
       <c r="V372" s="7"/>
     </row>
-    <row r="373" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A373" s="8"/>
       <c r="B373" s="4" t="s">
         <v>4</v>
@@ -36212,7 +36218,7 @@
       </c>
       <c r="V373" s="7"/>
     </row>
-    <row r="374" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A374" s="9"/>
       <c r="B374" s="4" t="s">
         <v>4</v>
@@ -36276,7 +36282,7 @@
       </c>
       <c r="V374" s="7"/>
     </row>
-    <row r="375" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A375" s="8"/>
       <c r="B375" s="4" t="s">
         <v>4</v>
@@ -36340,7 +36346,7 @@
       </c>
       <c r="V375" s="7"/>
     </row>
-    <row r="376" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A376" s="3" t="s">
         <v>21</v>
       </c>
@@ -36406,7 +36412,7 @@
       </c>
       <c r="V376" s="7"/>
     </row>
-    <row r="377" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A377" s="8"/>
       <c r="B377" s="4" t="s">
         <v>4</v>
@@ -36470,7 +36476,7 @@
       </c>
       <c r="V377" s="7"/>
     </row>
-    <row r="378" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A378" s="8"/>
       <c r="B378" s="4" t="s">
         <v>4</v>
@@ -36534,7 +36540,7 @@
       </c>
       <c r="V378" s="7"/>
     </row>
-    <row r="379" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A379" s="8"/>
       <c r="B379" s="4" t="s">
         <v>4</v>
@@ -36598,7 +36604,7 @@
       </c>
       <c r="V379" s="7"/>
     </row>
-    <row r="380" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A380" s="8"/>
       <c r="B380" s="4" t="s">
         <v>4</v>
@@ -36662,7 +36668,7 @@
       </c>
       <c r="V380" s="7"/>
     </row>
-    <row r="381" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A381" s="8"/>
       <c r="B381" s="4" t="s">
         <v>4</v>
@@ -36726,7 +36732,7 @@
       </c>
       <c r="V381" s="7"/>
     </row>
-    <row r="382" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A382" s="8"/>
       <c r="B382" s="4" t="s">
         <v>4</v>
@@ -36790,7 +36796,7 @@
       </c>
       <c r="V382" s="7"/>
     </row>
-    <row r="383" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A383" s="8"/>
       <c r="B383" s="4" t="s">
         <v>4</v>
@@ -36854,7 +36860,7 @@
       </c>
       <c r="V383" s="7"/>
     </row>
-    <row r="384" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A384" s="8"/>
       <c r="B384" s="4" t="s">
         <v>4</v>
@@ -36918,7 +36924,7 @@
       </c>
       <c r="V384" s="7"/>
     </row>
-    <row r="385" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A385" s="8"/>
       <c r="B385" s="4" t="s">
         <v>4</v>
@@ -36982,7 +36988,7 @@
       </c>
       <c r="V385" s="7"/>
     </row>
-    <row r="386" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A386" s="8"/>
       <c r="B386" s="4" t="s">
         <v>4</v>
@@ -37046,7 +37052,7 @@
       </c>
       <c r="V386" s="7"/>
     </row>
-    <row r="387" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A387" s="8"/>
       <c r="B387" s="4" t="s">
         <v>4</v>
@@ -37110,7 +37116,7 @@
       </c>
       <c r="V387" s="7"/>
     </row>
-    <row r="388" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A388" s="8"/>
       <c r="B388" s="4" t="s">
         <v>4</v>
@@ -37174,7 +37180,7 @@
       </c>
       <c r="V388" s="7"/>
     </row>
-    <row r="389" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A389" s="8"/>
       <c r="B389" s="4" t="s">
         <v>4</v>
@@ -37238,7 +37244,7 @@
       </c>
       <c r="V389" s="7"/>
     </row>
-    <row r="390" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A390" s="8"/>
       <c r="B390" s="4" t="s">
         <v>4</v>
@@ -37302,7 +37308,7 @@
       </c>
       <c r="V390" s="7"/>
     </row>
-    <row r="391" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A391" s="8"/>
       <c r="B391" s="4" t="s">
         <v>4</v>
@@ -37366,7 +37372,7 @@
       </c>
       <c r="V391" s="7"/>
     </row>
-    <row r="392" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A392" s="8"/>
       <c r="B392" s="4" t="s">
         <v>4</v>
@@ -37430,7 +37436,7 @@
       </c>
       <c r="V392" s="7"/>
     </row>
-    <row r="393" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A393" s="8"/>
       <c r="B393" s="4" t="s">
         <v>4</v>
@@ -37494,7 +37500,7 @@
       </c>
       <c r="V393" s="7"/>
     </row>
-    <row r="394" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A394" s="8"/>
       <c r="B394" s="4" t="s">
         <v>4</v>
@@ -37558,7 +37564,7 @@
       </c>
       <c r="V394" s="7"/>
     </row>
-    <row r="395" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A395" s="8"/>
       <c r="B395" s="4" t="s">
         <v>4</v>
@@ -37622,7 +37628,7 @@
       </c>
       <c r="V395" s="7"/>
     </row>
-    <row r="396" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A396" s="8"/>
       <c r="B396" s="4" t="s">
         <v>4</v>
@@ -37686,7 +37692,7 @@
       </c>
       <c r="V396" s="7"/>
     </row>
-    <row r="397" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A397" s="8"/>
       <c r="B397" s="4" t="s">
         <v>4</v>
@@ -37750,7 +37756,7 @@
       </c>
       <c r="V397" s="7"/>
     </row>
-    <row r="398" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A398" s="8"/>
       <c r="B398" s="4" t="s">
         <v>4</v>
@@ -37814,7 +37820,7 @@
       </c>
       <c r="V398" s="7"/>
     </row>
-    <row r="399" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A399" s="8"/>
       <c r="B399" s="4" t="s">
         <v>4</v>
@@ -37878,7 +37884,7 @@
       </c>
       <c r="V399" s="7"/>
     </row>
-    <row r="400" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A400" s="8"/>
       <c r="B400" s="4" t="s">
         <v>4</v>
@@ -37942,7 +37948,7 @@
       </c>
       <c r="V400" s="7"/>
     </row>
-    <row r="401" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A401" s="8"/>
       <c r="B401" s="4" t="s">
         <v>4</v>
@@ -38006,7 +38012,7 @@
       </c>
       <c r="V401" s="7"/>
     </row>
-    <row r="402" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A402" s="8"/>
       <c r="B402" s="4" t="s">
         <v>4</v>
@@ -38070,7 +38076,7 @@
       </c>
       <c r="V402" s="7"/>
     </row>
-    <row r="403" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A403" s="8"/>
       <c r="B403" s="4" t="s">
         <v>4</v>
@@ -38134,7 +38140,7 @@
       </c>
       <c r="V403" s="7"/>
     </row>
-    <row r="404" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A404" s="3" t="s">
         <v>20</v>
       </c>
@@ -38200,7 +38206,7 @@
       </c>
       <c r="V404" s="7"/>
     </row>
-    <row r="405" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A405" s="8"/>
       <c r="B405" s="4" t="s">
         <v>4</v>
@@ -38264,7 +38270,7 @@
       </c>
       <c r="V405" s="7"/>
     </row>
-    <row r="406" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A406" s="8"/>
       <c r="B406" s="4" t="s">
         <v>4</v>
@@ -38328,7 +38334,7 @@
       </c>
       <c r="V406" s="7"/>
     </row>
-    <row r="407" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A407" s="8"/>
       <c r="B407" s="4" t="s">
         <v>4</v>
@@ -38392,7 +38398,7 @@
       </c>
       <c r="V407" s="7"/>
     </row>
-    <row r="408" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A408" s="8"/>
       <c r="B408" s="4" t="s">
         <v>4</v>
@@ -38456,7 +38462,7 @@
       </c>
       <c r="V408" s="7"/>
     </row>
-    <row r="409" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A409" s="8"/>
       <c r="B409" s="4" t="s">
         <v>4</v>
@@ -38520,7 +38526,7 @@
       </c>
       <c r="V409" s="7"/>
     </row>
-    <row r="410" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A410" s="8"/>
       <c r="B410" s="4" t="s">
         <v>4</v>
@@ -38584,7 +38590,7 @@
       </c>
       <c r="V410" s="7"/>
     </row>
-    <row r="411" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A411" s="8"/>
       <c r="B411" s="4" t="s">
         <v>4</v>
@@ -38648,7 +38654,7 @@
       </c>
       <c r="V411" s="7"/>
     </row>
-    <row r="412" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A412" s="8"/>
       <c r="B412" s="4" t="s">
         <v>4</v>
@@ -38712,7 +38718,7 @@
       </c>
       <c r="V412" s="7"/>
     </row>
-    <row r="413" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A413" s="8"/>
       <c r="B413" s="4" t="s">
         <v>4</v>
@@ -38776,7 +38782,7 @@
       </c>
       <c r="V413" s="7"/>
     </row>
-    <row r="414" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A414" s="8"/>
       <c r="B414" s="4" t="s">
         <v>4</v>
@@ -38840,7 +38846,7 @@
       </c>
       <c r="V414" s="7"/>
     </row>
-    <row r="415" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A415" s="8"/>
       <c r="B415" s="4" t="s">
         <v>4</v>
@@ -38904,7 +38910,7 @@
       </c>
       <c r="V415" s="7"/>
     </row>
-    <row r="416" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A416" s="9"/>
       <c r="B416" s="4" t="s">
         <v>4</v>
@@ -38968,7 +38974,7 @@
       </c>
       <c r="V416" s="7"/>
     </row>
-    <row r="417" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A417" s="8"/>
       <c r="B417" s="4" t="s">
         <v>4</v>
@@ -39032,7 +39038,7 @@
       </c>
       <c r="V417" s="7"/>
     </row>
-    <row r="418" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A418" s="8"/>
       <c r="B418" s="4" t="s">
         <v>4</v>
@@ -39096,7 +39102,7 @@
       </c>
       <c r="V418" s="7"/>
     </row>
-    <row r="419" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A419" s="8"/>
       <c r="B419" s="4" t="s">
         <v>4</v>
@@ -39160,7 +39166,7 @@
       </c>
       <c r="V419" s="7"/>
     </row>
-    <row r="420" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A420" s="8"/>
       <c r="B420" s="4" t="s">
         <v>4</v>
@@ -39224,7 +39230,7 @@
       </c>
       <c r="V420" s="7"/>
     </row>
-    <row r="421" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A421" s="8"/>
       <c r="B421" s="4" t="s">
         <v>4</v>
@@ -39288,7 +39294,7 @@
       </c>
       <c r="V421" s="7"/>
     </row>
-    <row r="422" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A422" s="8"/>
       <c r="B422" s="4" t="s">
         <v>4</v>
@@ -39352,7 +39358,7 @@
       </c>
       <c r="V422" s="7"/>
     </row>
-    <row r="423" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A423" s="8"/>
       <c r="B423" s="4" t="s">
         <v>4</v>
@@ -39416,7 +39422,7 @@
       </c>
       <c r="V423" s="7"/>
     </row>
-    <row r="424" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A424" s="8"/>
       <c r="B424" s="4" t="s">
         <v>4</v>
@@ -39480,7 +39486,7 @@
       </c>
       <c r="V424" s="7"/>
     </row>
-    <row r="425" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A425" s="8"/>
       <c r="B425" s="4" t="s">
         <v>4</v>
@@ -39544,7 +39550,7 @@
       </c>
       <c r="V425" s="7"/>
     </row>
-    <row r="426" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A426" s="8"/>
       <c r="B426" s="4" t="s">
         <v>4</v>
@@ -39608,7 +39614,7 @@
       </c>
       <c r="V426" s="7"/>
     </row>
-    <row r="427" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A427" s="8"/>
       <c r="B427" s="4" t="s">
         <v>4</v>
@@ -39672,7 +39678,7 @@
       </c>
       <c r="V427" s="7"/>
     </row>
-    <row r="428" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A428" s="8"/>
       <c r="B428" s="4" t="s">
         <v>4</v>
@@ -39736,7 +39742,7 @@
       </c>
       <c r="V428" s="7"/>
     </row>
-    <row r="429" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A429" s="8"/>
       <c r="B429" s="4" t="s">
         <v>4</v>
@@ -39800,7 +39806,7 @@
       </c>
       <c r="V429" s="7"/>
     </row>
-    <row r="430" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A430" s="8"/>
       <c r="B430" s="4" t="s">
         <v>4</v>
@@ -39864,7 +39870,7 @@
       </c>
       <c r="V430" s="7"/>
     </row>
-    <row r="431" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A431" s="8"/>
       <c r="B431" s="4" t="s">
         <v>4</v>
@@ -39928,7 +39934,7 @@
       </c>
       <c r="V431" s="7"/>
     </row>
-    <row r="432" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A432" s="8"/>
       <c r="B432" s="4" t="s">
         <v>4</v>
@@ -39992,7 +39998,7 @@
       </c>
       <c r="V432" s="7"/>
     </row>
-    <row r="433" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A433" s="8"/>
       <c r="B433" s="4" t="s">
         <v>4</v>
@@ -40056,7 +40062,7 @@
       </c>
       <c r="V433" s="7"/>
     </row>
-    <row r="434" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A434" s="8"/>
       <c r="B434" s="4" t="s">
         <v>4</v>
@@ -40120,7 +40126,7 @@
       </c>
       <c r="V434" s="7"/>
     </row>
-    <row r="435" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A435" s="8"/>
       <c r="B435" s="4" t="s">
         <v>4</v>
@@ -40184,7 +40190,7 @@
       </c>
       <c r="V435" s="7"/>
     </row>
-    <row r="436" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A436" s="9"/>
       <c r="B436" s="4" t="s">
         <v>4</v>
@@ -40248,7 +40254,7 @@
       </c>
       <c r="V436" s="7"/>
     </row>
-    <row r="437" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A437" s="8"/>
       <c r="B437" s="4" t="s">
         <v>4</v>
@@ -40312,7 +40318,7 @@
       </c>
       <c r="V437" s="7"/>
     </row>
-    <row r="438" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A438" s="8"/>
       <c r="B438" s="4" t="s">
         <v>4</v>
@@ -40376,7 +40382,7 @@
       </c>
       <c r="V438" s="7"/>
     </row>
-    <row r="439" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A439" s="8"/>
       <c r="B439" s="4" t="s">
         <v>4</v>
@@ -40440,7 +40446,7 @@
       </c>
       <c r="V439" s="7"/>
     </row>
-    <row r="440" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A440" s="8"/>
       <c r="B440" s="4" t="s">
         <v>4</v>
@@ -40504,7 +40510,7 @@
       </c>
       <c r="V440" s="7"/>
     </row>
-    <row r="441" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A441" s="3" t="s">
         <v>19</v>
       </c>
@@ -40570,7 +40576,7 @@
       </c>
       <c r="V441" s="7"/>
     </row>
-    <row r="442" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A442" s="8"/>
       <c r="B442" s="4" t="s">
         <v>4</v>
@@ -40634,7 +40640,7 @@
       </c>
       <c r="V442" s="7"/>
     </row>
-    <row r="443" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A443" s="8"/>
       <c r="B443" s="4" t="s">
         <v>4</v>
@@ -40698,7 +40704,7 @@
       </c>
       <c r="V443" s="7"/>
     </row>
-    <row r="444" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A444" s="8"/>
       <c r="B444" s="4" t="s">
         <v>4</v>
@@ -40762,7 +40768,7 @@
       </c>
       <c r="V444" s="7"/>
     </row>
-    <row r="445" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A445" s="8"/>
       <c r="B445" s="4" t="s">
         <v>4</v>
@@ -40826,7 +40832,7 @@
       </c>
       <c r="V445" s="7"/>
     </row>
-    <row r="446" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A446" s="8"/>
       <c r="B446" s="4" t="s">
         <v>4</v>
@@ -40890,7 +40896,7 @@
       </c>
       <c r="V446" s="7"/>
     </row>
-    <row r="447" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A447" s="8"/>
       <c r="B447" s="4" t="s">
         <v>4</v>
@@ -40954,7 +40960,7 @@
       </c>
       <c r="V447" s="7"/>
     </row>
-    <row r="448" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A448" s="8"/>
       <c r="B448" s="4" t="s">
         <v>4</v>
@@ -41018,7 +41024,7 @@
       </c>
       <c r="V448" s="7"/>
     </row>
-    <row r="449" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A449" s="8"/>
       <c r="B449" s="4" t="s">
         <v>4</v>
@@ -41082,7 +41088,7 @@
       </c>
       <c r="V449" s="7"/>
     </row>
-    <row r="450" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A450" s="8"/>
       <c r="B450" s="4" t="s">
         <v>4</v>
@@ -41146,7 +41152,7 @@
       </c>
       <c r="V450" s="7"/>
     </row>
-    <row r="451" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A451" s="8"/>
       <c r="B451" s="4" t="s">
         <v>4</v>
@@ -41210,7 +41216,7 @@
       </c>
       <c r="V451" s="7"/>
     </row>
-    <row r="452" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A452" s="8"/>
       <c r="B452" s="4" t="s">
         <v>4</v>
@@ -41274,7 +41280,7 @@
       </c>
       <c r="V452" s="7"/>
     </row>
-    <row r="453" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A453" s="8"/>
       <c r="B453" s="4" t="s">
         <v>4</v>
@@ -41338,7 +41344,7 @@
       </c>
       <c r="V453" s="7"/>
     </row>
-    <row r="454" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A454" s="8"/>
       <c r="B454" s="4" t="s">
         <v>4</v>
@@ -41402,7 +41408,7 @@
       </c>
       <c r="V454" s="7"/>
     </row>
-    <row r="455" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A455" s="8"/>
       <c r="B455" s="4" t="s">
         <v>4</v>
@@ -41466,7 +41472,7 @@
       </c>
       <c r="V455" s="7"/>
     </row>
-    <row r="456" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A456" s="8"/>
       <c r="B456" s="4" t="s">
         <v>4</v>
@@ -41530,7 +41536,7 @@
       </c>
       <c r="V456" s="7"/>
     </row>
-    <row r="457" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A457" s="8"/>
       <c r="B457" s="4" t="s">
         <v>4</v>
@@ -41594,7 +41600,7 @@
       </c>
       <c r="V457" s="7"/>
     </row>
-    <row r="458" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A458" s="8"/>
       <c r="B458" s="4" t="s">
         <v>4</v>
@@ -41658,7 +41664,7 @@
       </c>
       <c r="V458" s="7"/>
     </row>
-    <row r="459" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A459" s="8"/>
       <c r="B459" s="4" t="s">
         <v>4</v>
@@ -41722,7 +41728,7 @@
       </c>
       <c r="V459" s="7"/>
     </row>
-    <row r="460" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A460" s="8"/>
       <c r="B460" s="4" t="s">
         <v>4</v>
@@ -41786,7 +41792,7 @@
       </c>
       <c r="V460" s="7"/>
     </row>
-    <row r="461" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A461" s="8"/>
       <c r="B461" s="4" t="s">
         <v>4</v>
@@ -41850,7 +41856,7 @@
       </c>
       <c r="V461" s="7"/>
     </row>
-    <row r="462" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A462" s="9"/>
       <c r="B462" s="4" t="s">
         <v>4</v>
@@ -41914,7 +41920,7 @@
       </c>
       <c r="V462" s="7"/>
     </row>
-    <row r="463" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A463" s="8"/>
       <c r="B463" s="4" t="s">
         <v>4</v>
@@ -41978,7 +41984,7 @@
       </c>
       <c r="V463" s="7"/>
     </row>
-    <row r="464" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A464" s="8"/>
       <c r="B464" s="4" t="s">
         <v>4</v>
@@ -42042,7 +42048,7 @@
       </c>
       <c r="V464" s="7"/>
     </row>
-    <row r="465" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A465" s="8"/>
       <c r="B465" s="4" t="s">
         <v>4</v>
@@ -42106,7 +42112,7 @@
       </c>
       <c r="V465" s="7"/>
     </row>
-    <row r="466" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A466" s="8"/>
       <c r="B466" s="4" t="s">
         <v>4</v>
@@ -42170,7 +42176,7 @@
       </c>
       <c r="V466" s="7"/>
     </row>
-    <row r="467" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A467" s="8"/>
       <c r="B467" s="4" t="s">
         <v>4</v>
@@ -42234,7 +42240,7 @@
       </c>
       <c r="V467" s="7"/>
     </row>
-    <row r="468" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A468" s="8"/>
       <c r="B468" s="4" t="s">
         <v>4</v>
@@ -42298,7 +42304,7 @@
       </c>
       <c r="V468" s="7"/>
     </row>
-    <row r="469" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A469" s="8"/>
       <c r="B469" s="4" t="s">
         <v>4</v>
@@ -42362,7 +42368,7 @@
       </c>
       <c r="V469" s="7"/>
     </row>
-    <row r="470" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A470" s="8"/>
       <c r="B470" s="4" t="s">
         <v>4</v>
@@ -42426,7 +42432,7 @@
       </c>
       <c r="V470" s="7"/>
     </row>
-    <row r="471" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A471" s="8"/>
       <c r="B471" s="4" t="s">
         <v>4</v>
@@ -42490,7 +42496,7 @@
       </c>
       <c r="V471" s="7"/>
     </row>
-    <row r="472" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A472" s="8"/>
       <c r="B472" s="4" t="s">
         <v>4</v>
@@ -42554,7 +42560,7 @@
       </c>
       <c r="V472" s="7"/>
     </row>
-    <row r="473" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A473" s="3" t="s">
         <v>17</v>
       </c>
@@ -42620,7 +42626,7 @@
       </c>
       <c r="V473" s="7"/>
     </row>
-    <row r="474" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A474" s="8"/>
       <c r="B474" s="4" t="s">
         <v>4</v>
@@ -42684,7 +42690,7 @@
       </c>
       <c r="V474" s="7"/>
     </row>
-    <row r="475" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A475" s="8"/>
       <c r="B475" s="4" t="s">
         <v>4</v>
@@ -42748,7 +42754,7 @@
       </c>
       <c r="V475" s="7"/>
     </row>
-    <row r="476" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A476" s="8"/>
       <c r="B476" s="4" t="s">
         <v>4</v>
@@ -42812,7 +42818,7 @@
       </c>
       <c r="V476" s="7"/>
     </row>
-    <row r="477" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A477" s="8"/>
       <c r="B477" s="4" t="s">
         <v>4</v>
@@ -42876,7 +42882,7 @@
       </c>
       <c r="V477" s="7"/>
     </row>
-    <row r="478" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A478" s="9"/>
       <c r="B478" s="4" t="s">
         <v>4</v>
@@ -42940,7 +42946,7 @@
       </c>
       <c r="V478" s="7"/>
     </row>
-    <row r="479" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A479" s="8"/>
       <c r="B479" s="4" t="s">
         <v>4</v>
@@ -43004,7 +43010,7 @@
       </c>
       <c r="V479" s="7"/>
     </row>
-    <row r="480" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A480" s="8"/>
       <c r="B480" s="4" t="s">
         <v>4</v>
@@ -43068,7 +43074,7 @@
       </c>
       <c r="V480" s="7"/>
     </row>
-    <row r="481" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A481" s="8"/>
       <c r="B481" s="4" t="s">
         <v>4</v>
@@ -43132,7 +43138,7 @@
       </c>
       <c r="V481" s="7"/>
     </row>
-    <row r="482" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A482" s="8"/>
       <c r="B482" s="4" t="s">
         <v>4</v>
@@ -43196,7 +43202,7 @@
       </c>
       <c r="V482" s="7"/>
     </row>
-    <row r="483" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A483" s="8"/>
       <c r="B483" s="4" t="s">
         <v>4</v>
@@ -43260,7 +43266,7 @@
       </c>
       <c r="V483" s="7"/>
     </row>
-    <row r="484" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A484" s="8"/>
       <c r="B484" s="4" t="s">
         <v>4</v>
@@ -43324,7 +43330,7 @@
       </c>
       <c r="V484" s="7"/>
     </row>
-    <row r="485" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A485" s="8"/>
       <c r="B485" s="4" t="s">
         <v>4</v>
@@ -43388,7 +43394,7 @@
       </c>
       <c r="V485" s="7"/>
     </row>
-    <row r="486" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A486" s="8"/>
       <c r="B486" s="4" t="s">
         <v>4</v>
@@ -43452,7 +43458,7 @@
       </c>
       <c r="V486" s="7"/>
     </row>
-    <row r="487" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A487" s="8"/>
       <c r="B487" s="4" t="s">
         <v>4</v>
@@ -43516,7 +43522,7 @@
       </c>
       <c r="V487" s="7"/>
     </row>
-    <row r="488" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A488" s="9"/>
       <c r="B488" s="4" t="s">
         <v>4</v>
@@ -43580,7 +43586,7 @@
       </c>
       <c r="V488" s="7"/>
     </row>
-    <row r="489" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A489" s="8"/>
       <c r="B489" s="4" t="s">
         <v>4</v>
@@ -43644,7 +43650,7 @@
       </c>
       <c r="V489" s="7"/>
     </row>
-    <row r="490" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A490" s="8"/>
       <c r="B490" s="4" t="s">
         <v>4</v>
@@ -43708,7 +43714,7 @@
       </c>
       <c r="V490" s="7"/>
     </row>
-    <row r="491" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A491" s="8"/>
       <c r="B491" s="4" t="s">
         <v>4</v>
@@ -43772,7 +43778,7 @@
       </c>
       <c r="V491" s="7"/>
     </row>
-    <row r="492" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A492" s="8"/>
       <c r="B492" s="4" t="s">
         <v>4</v>
@@ -43836,7 +43842,7 @@
       </c>
       <c r="V492" s="7"/>
     </row>
-    <row r="493" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A493" s="8"/>
       <c r="B493" s="4" t="s">
         <v>4</v>
@@ -43900,7 +43906,7 @@
       </c>
       <c r="V493" s="7"/>
     </row>
-    <row r="494" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:22" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A494" s="8"/>
       <c r="B494" s="4" t="s">
         <v>4</v>

</xml_diff>